<commit_message>
fix dev of alliance&mail
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6260" yWindow="22260" windowWidth="27520" windowHeight="14540" tabRatio="883" activeTab="1"/>
+    <workbookView xWindow="5680" yWindow="22260" windowWidth="27520" windowHeight="14540" tabRatio="883" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="resources" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="24">
   <si>
     <t>INT_level</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -40,34 +40,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>STR_editAllianceNotice</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>STR_editAllianceDescription</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>STR_modifyAllianceMemberTitle</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>STR_kickAllianceMemberOff</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>STR_handOverArchon</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>STR_sendAllianceMail</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>STR_handleJoinAllianceRequest</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>true</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -76,10 +48,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>STR_editAllianceBasicInfo</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>archon</t>
   </si>
   <si>
@@ -109,7 +77,47 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>STR_editTitleName</t>
+    <t>BOOL_editTitleName</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_editAllianceBasicInfo</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_editAllianceNotice</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_editAllianceDescription</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_modifyAllianceMemberTitle</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_kickAllianceMemberOff</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_handOverArchon</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_sendAllianceMail</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_handleJoinAllianceRequest</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_editAllianceJoinType</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_inviteToJoinAlliance</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -259,7 +267,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="60">
+  <cellStyleXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -274,6 +282,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -349,7 +361,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="60">
+  <cellStyles count="64">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -382,6 +394,8 @@
     <cellStyle name="超链接" xfId="54" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="56" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="62" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -407,6 +421,8 @@
     <cellStyle name="访问过的超链接" xfId="55" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="57" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -904,10 +920,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -917,284 +933,332 @@
     <col min="6" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="L1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="M1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="20" customHeight="1">
+      <c r="A2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="20" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="20" customHeight="1">
+    <row r="3" spans="1:13" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="20" customHeight="1">
+    <row r="4" spans="1:13" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="20" customHeight="1">
+    <row r="5" spans="1:13" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="20" customHeight="1">
+    <row r="6" spans="1:13" ht="20" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="20" customHeight="1">
+    <row r="7" spans="1:13" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="20" customHeight="1">
+      <c r="A8" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="20" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bugfix for alliance speedup
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="23">
   <si>
     <t>INT_level</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>general</t>
-  </si>
-  <si>
-    <t>diplomat</t>
   </si>
   <si>
     <t>quartermaster</t>
@@ -920,10 +917,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:M8"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -935,43 +932,43 @@
   <sheetData>
     <row r="1" spans="1:13" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="20" customHeight="1">
@@ -1061,7 +1058,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>3</v>
@@ -1102,7 +1099,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>3</v>
@@ -1143,7 +1140,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>3</v>
@@ -1184,7 +1181,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>3</v>
@@ -1217,47 +1214,6 @@
         <v>3</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="20" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1">
-        <v>7</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="M8" s="7" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finish dev of donate alliance
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10060" yWindow="5120" windowWidth="27520" windowHeight="14540" tabRatio="883" activeTab="3"/>
+    <workbookView xWindow="6280" yWindow="2800" windowWidth="27520" windowHeight="14540" tabRatio="883" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="resource" sheetId="2" r:id="rId1"/>
@@ -12,9 +12,6 @@
     <sheet name="buildingType" sheetId="6" r:id="rId3"/>
     <sheet name="donate" sheetId="8" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <definedNames>
     <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="2">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="3">#REF!</definedName>
@@ -43,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="87">
   <si>
     <t>INT_gem</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -379,6 +376,10 @@
   </si>
   <si>
     <t>STR_resource</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>wood_1m</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -541,7 +542,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="110">
+  <cellStyleXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -556,6 +557,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -693,7 +698,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="110">
+  <cellStyles count="114">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -751,6 +756,8 @@
     <cellStyle name="超链接" xfId="104" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="106" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="112" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -801,6 +808,8 @@
     <cellStyle name="访问过的超链接" xfId="105" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="107" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="113" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -876,12 +885,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1837,8 +1840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2025,10 +2028,10 @@
     </row>
     <row r="7" spans="1:16" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C7" s="1">
         <v>6</v>
@@ -2213,10 +2216,10 @@
     </row>
     <row r="13" spans="1:16" ht="20" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" s="1">
         <v>6</v>

</xml_diff>

<commit_message>
finish dev of distroyAllianceDecorate
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8620" yWindow="2140" windowWidth="27520" windowHeight="14540" tabRatio="883"/>
+    <workbookView xWindow="7860" yWindow="4220" windowWidth="27520" windowHeight="14540" tabRatio="883" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="resource" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="110">
   <si>
     <t>INT_gem</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -464,6 +464,14 @@
   </si>
   <si>
     <t>BOOL_moveAllianceBuilding</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_distroyNeedHonour</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_distroyAllianceDecorate</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -626,7 +634,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="148">
+  <cellStyleXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -641,6 +649,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -816,7 +826,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="148">
+  <cellStyles count="150">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -893,6 +903,7 @@
     <cellStyle name="超链接" xfId="142" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="144" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="148" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -962,6 +973,7 @@
     <cellStyle name="访问过的超链接" xfId="143" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="145" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="149" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -1413,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1492,10 +1504,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1507,7 +1519,7 @@
     <col min="14" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -1556,8 +1568,11 @@
       <c r="P1" s="3" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="20" customHeight="1">
+      <c r="Q1" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1606,8 +1621,11 @@
       <c r="P2" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="20" customHeight="1">
+      <c r="Q2" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1656,8 +1674,11 @@
       <c r="P3" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" ht="20" customHeight="1">
+      <c r="Q3" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1706,8 +1727,11 @@
       <c r="P4" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" ht="20" customHeight="1">
+      <c r="Q4" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1756,8 +1780,11 @@
       <c r="P5" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="20" customHeight="1">
+      <c r="Q5" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="20" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1806,8 +1833,11 @@
       <c r="P6" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="20" customHeight="1">
+      <c r="Q6" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1856,8 +1886,11 @@
       <c r="P7" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="20" customHeight="1">
+      <c r="Q7" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="20" customHeight="1">
       <c r="M8" s="7"/>
     </row>
   </sheetData>
@@ -1877,7 +1910,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1885,7 +1918,7 @@
     <col min="1" max="2" width="20.6640625" style="1"/>
     <col min="3" max="3" width="20.6640625" style="8"/>
     <col min="4" max="4" width="20.6640625" style="1"/>
-    <col min="5" max="5" width="20.6640625" style="6"/>
+    <col min="5" max="5" width="20.6640625" style="8"/>
     <col min="6" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
@@ -1902,7 +1935,9 @@
       <c r="D1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="5"/>
+      <c r="E1" s="10" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="2" spans="1:13" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -1916,6 +1951,9 @@
       </c>
       <c r="D2" s="1" t="s">
         <v>95</v>
+      </c>
+      <c r="E2" s="8">
+        <v>120</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -1938,6 +1976,9 @@
       <c r="D3" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="E3" s="8">
+        <v>80</v>
+      </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -1959,6 +2000,9 @@
       <c r="D4" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="E4" s="8">
+        <v>40</v>
+      </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -1980,6 +2024,9 @@
       <c r="D5" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="E5" s="8">
+        <v>20</v>
+      </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -2001,6 +2048,9 @@
       <c r="D6" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="E6" s="8">
+        <v>20</v>
+      </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -2022,6 +2072,9 @@
       <c r="D7" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="E7" s="8">
+        <v>20</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -2043,7 +2096,9 @@
       <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -2066,7 +2121,9 @@
       <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -2089,7 +2146,9 @@
       <c r="D10" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
@@ -2112,6 +2171,9 @@
       <c r="D11" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="E11" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:13" ht="20" customHeight="1">
       <c r="A12" s="1" t="s">
@@ -2126,6 +2188,9 @@
       <c r="D12" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="20" customHeight="1">
       <c r="A13" s="1" t="s">
@@ -2140,6 +2205,9 @@
       <c r="D13" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="E13" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:13" ht="20" customHeight="1">
       <c r="A14" s="1" t="s">
@@ -2153,6 +2221,9 @@
       </c>
       <c r="D14" s="1" t="s">
         <v>96</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dev of alliance shrine
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6680" yWindow="5680" windowWidth="27520" windowHeight="14540" tabRatio="883" activeTab="2"/>
+    <workbookView xWindow="7000" yWindow="3300" windowWidth="27520" windowHeight="14540" tabRatio="883" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="resource" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="111">
   <si>
     <t>INT_gem</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -472,6 +472,10 @@
   </si>
   <si>
     <t>INT_distroyNeedHonour</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_activateAllianceShrineStage</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -634,7 +638,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="158">
+  <cellStyleXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -649,6 +653,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -834,7 +840,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="158">
+  <cellStyles count="160">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -916,6 +922,7 @@
     <cellStyle name="超链接" xfId="152" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="154" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="158" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -990,6 +997,7 @@
     <cellStyle name="访问过的超链接" xfId="153" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="155" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="159" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -1520,10 +1528,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:Q7"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2:R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1535,7 +1543,7 @@
     <col min="14" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -1587,8 +1595,11 @@
       <c r="Q1" s="3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" ht="20" customHeight="1">
+      <c r="R1" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1640,8 +1651,11 @@
       <c r="Q2" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="20" customHeight="1">
+      <c r="R2" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1693,8 +1707,11 @@
       <c r="Q3" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="20" customHeight="1">
+      <c r="R3" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1746,8 +1763,11 @@
       <c r="Q4" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" ht="20" customHeight="1">
+      <c r="R4" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1799,8 +1819,11 @@
       <c r="Q5" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" ht="20" customHeight="1">
+      <c r="R5" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="20" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1852,8 +1875,11 @@
       <c r="Q6" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" ht="20" customHeight="1">
+      <c r="R6" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1905,8 +1931,11 @@
       <c r="Q7" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" ht="20" customHeight="1">
+      <c r="R7" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="20" customHeight="1">
       <c r="M8" s="7"/>
     </row>
   </sheetData>
@@ -1925,7 +1954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
dev of alliance shrine stage
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,34 +4,39 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7000" yWindow="3300" windowWidth="27520" windowHeight="14540" tabRatio="883" activeTab="1"/>
+    <workbookView xWindow="10380" yWindow="4080" windowWidth="27520" windowHeight="14540" tabRatio="883"/>
   </bookViews>
   <sheets>
-    <sheet name="resource" sheetId="2" r:id="rId1"/>
-    <sheet name="right" sheetId="4" r:id="rId2"/>
-    <sheet name="buildingType" sheetId="6" r:id="rId3"/>
-    <sheet name="donate" sheetId="8" r:id="rId4"/>
-    <sheet name="decorateCount" sheetId="9" r:id="rId5"/>
+    <sheet name="intInit" sheetId="2" r:id="rId1"/>
+    <sheet name="stringInit" sheetId="10" r:id="rId2"/>
+    <sheet name="right" sheetId="4" r:id="rId3"/>
+    <sheet name="buildingType" sheetId="6" r:id="rId4"/>
+    <sheet name="donate" sheetId="8" r:id="rId5"/>
+    <sheet name="decorateCount" sheetId="9" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="3">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="5">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="4">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="2">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="4">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="3">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="1">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="3">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="5">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="4">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="2">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="4">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="3">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="1">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_6">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="3">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="5">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="4">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="2">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="4">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="3">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="1">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_7">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="3">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="5">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="4">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="2">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="4">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="3">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="1">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_8">#REF!</definedName>
   </definedNames>
@@ -45,11 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="111">
-  <si>
-    <t>INT_gem</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="112">
   <si>
     <t>true</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -121,361 +122,369 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
+    <t>buyArchon</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>member</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>building</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>decorate_tree_2</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>decorate_tree_1</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>decorate_mountain_2</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>decorate_mountain_1</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>decorate_lake_2</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>decorate_lake_1</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_height</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_width</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR_type</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_loyalty</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_honour</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>FLOAT_extra</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>wood_20k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>wood_50k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>wood_100k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>wood_500k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>stone_1m</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>stone_20k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>stone_50k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>stone_100k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>stone_500k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>iron_1m</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>iron_20k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>iron_50k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>iron_100k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>iron_500k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>food_20k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>food_50k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>food_100k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>food_500k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>food_1m</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>coin_20k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>coin_50k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>coin_100k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>coin_500k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>coin_1m</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>gem_20</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>gem_50</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>gem_100</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>gem_500</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>gem_1000</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_level</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>wood_200k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>stone_200k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>iron_200k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>food_200k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>coin_200k</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>gem_200</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>wood</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>wood</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>stone</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>iron</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>food</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>coin</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>gem</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR_type</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_count</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR_resource</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>wood_1m</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>false</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_upgradeAllianceBuilding</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_editAllianceTerrian</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>editAllianceBasicInfo</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>editAllianceTerrian</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_upgradeAllianceVillage</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>woodVillage</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>stoneVillage</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>ironVillage</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>foodVillage</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>coinVillage</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>decorate</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>village</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR_category</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>decorate_lake_1</t>
+  </si>
+  <si>
+    <t>decorate_lake_2</t>
+  </si>
+  <si>
+    <t>decorate_mountain_1</t>
+  </si>
+  <si>
+    <t>decorate_mountain_2</t>
+  </si>
+  <si>
+    <t>decorate_tree_1</t>
+  </si>
+  <si>
+    <t>decorate_tree_2</t>
+  </si>
+  <si>
+    <t>INT_count</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_editAllianceTitleName</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_editAllianceMemberTitle</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_moveAllianceBuilding</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_distroyAllianceDecorate</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_distroyNeedHonour</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_activateAllianceShrineStage</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>activeShrineStageEvent</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR_value</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_value</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
     <t>createAlliance</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>buyArchon</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>member</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>building</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>decorate_tree_2</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>decorate_tree_1</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>decorate_mountain_2</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>decorate_mountain_1</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>decorate_lake_2</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>decorate_lake_1</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_height</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_width</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>STR_type</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_loyalty</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_honour</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>FLOAT_extra</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>wood_20k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>wood_50k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>wood_100k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>wood_500k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>stone_1m</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>stone_20k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>stone_50k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>stone_100k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>stone_500k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>iron_1m</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>iron_20k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>iron_50k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>iron_100k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>iron_500k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>food_20k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>food_50k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>food_100k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>food_500k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>food_1m</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>coin_20k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>coin_50k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>coin_100k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>coin_500k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>coin_1m</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>gem_20</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>gem_50</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>gem_100</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>gem_500</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>gem_1000</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_level</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>wood_200k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>stone_200k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>iron_200k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>food_200k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>coin_200k</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>gem_200</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>wood</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>wood</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>stone</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>iron</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>food</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>coin</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>gem</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>STR_type</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_count</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>STR_resource</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>wood_1m</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>false</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOOL_upgradeAllianceBuilding</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOOL_editAllianceTerrian</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>editAllianceBasicInfo</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>editAllianceTerrian</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_honour</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOOL_upgradeAllianceVillage</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>woodVillage</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>stoneVillage</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>ironVillage</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>foodVillage</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>coinVillage</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>decorate</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>village</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>STR_category</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>decorate_lake_1</t>
-  </si>
-  <si>
-    <t>decorate_lake_2</t>
-  </si>
-  <si>
-    <t>decorate_mountain_1</t>
-  </si>
-  <si>
-    <t>decorate_mountain_2</t>
-  </si>
-  <si>
-    <t>decorate_tree_1</t>
-  </si>
-  <si>
-    <t>decorate_tree_2</t>
-  </si>
-  <si>
-    <t>INT_count</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOOL_editAllianceTitleName</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOOL_editAllianceMemberTitle</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOOL_moveAllianceBuilding</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOOL_distroyAllianceDecorate</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_distroyNeedHonour</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOOL_activateAllianceShrineStage</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -638,7 +647,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="160">
+  <cellStyleXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -653,6 +662,28 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -840,7 +871,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="160">
+  <cellStyles count="182">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -923,6 +954,17 @@
     <cellStyle name="超链接" xfId="154" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="156" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="180" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -998,6 +1040,17 @@
     <cellStyle name="访问过的超链接" xfId="155" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="157" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="181" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -1447,10 +1500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1458,60 +1511,50 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" ht="20" customHeight="1">
+        <v>110</v>
+      </c>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="B2" s="1">
         <v>50</v>
       </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="20" customHeight="1">
+    </row>
+    <row r="3" spans="1:6" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2">
         <v>100</v>
       </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="20" customHeight="1">
+    </row>
+    <row r="4" spans="1:6" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4" s="2">
         <v>50</v>
       </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="20" customHeight="1">
+    </row>
+    <row r="5" spans="1:6" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>200</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="20" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1528,9 +1571,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="16384" width="20.6640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="B4" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="R2" sqref="R2:R7"/>
     </sheetView>
   </sheetViews>
@@ -1545,394 +1628,394 @@
   <sheetData>
     <row r="1" spans="1:18" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="20" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P7" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R7" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="20" customHeight="1">
@@ -1950,7 +2033,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
@@ -1969,24 +2052,24 @@
   <sheetData>
     <row r="1" spans="1:13" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1">
         <v>3</v>
@@ -1995,7 +2078,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E2" s="8">
         <v>120</v>
@@ -2010,7 +2093,7 @@
     </row>
     <row r="3" spans="1:13" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -2019,7 +2102,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E3" s="8">
         <v>80</v>
@@ -2034,7 +2117,7 @@
     </row>
     <row r="4" spans="1:13" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -2043,7 +2126,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E4" s="8">
         <v>40</v>
@@ -2058,7 +2141,7 @@
     </row>
     <row r="5" spans="1:13" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -2067,7 +2150,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E5" s="8">
         <v>20</v>
@@ -2082,7 +2165,7 @@
     </row>
     <row r="6" spans="1:13" ht="20" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -2091,7 +2174,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E6" s="8">
         <v>20</v>
@@ -2106,7 +2189,7 @@
     </row>
     <row r="7" spans="1:13" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -2115,7 +2198,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E7" s="8">
         <v>20</v>
@@ -2130,7 +2213,7 @@
     </row>
     <row r="8" spans="1:13" ht="20" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1">
         <v>3</v>
@@ -2139,7 +2222,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E8" s="9">
         <v>0</v>
@@ -2155,7 +2238,7 @@
     </row>
     <row r="9" spans="1:13" ht="20" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -2164,7 +2247,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E9" s="9">
         <v>0</v>
@@ -2180,7 +2263,7 @@
     </row>
     <row r="10" spans="1:13" ht="20" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -2189,7 +2272,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E10" s="9">
         <v>0</v>
@@ -2205,7 +2288,7 @@
     </row>
     <row r="11" spans="1:13" ht="20" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -2214,7 +2297,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E11" s="8">
         <v>0</v>
@@ -2222,7 +2305,7 @@
     </row>
     <row r="12" spans="1:13" ht="20" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -2231,7 +2314,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E12" s="8">
         <v>0</v>
@@ -2239,16 +2322,16 @@
     </row>
     <row r="13" spans="1:13" ht="20" customHeight="1">
       <c r="A13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="9">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="9">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="E13" s="8">
         <v>0</v>
@@ -2256,7 +2339,7 @@
     </row>
     <row r="14" spans="1:13" ht="20" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -2265,7 +2348,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E14" s="8">
         <v>0</v>
@@ -2283,7 +2366,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P37"/>
   <sheetViews>
@@ -2301,34 +2384,34 @@
   <sheetData>
     <row r="1" spans="1:16" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:16" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -2355,10 +2438,10 @@
     </row>
     <row r="3" spans="1:16" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -2385,10 +2468,10 @@
     </row>
     <row r="4" spans="1:16" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
@@ -2415,10 +2498,10 @@
     </row>
     <row r="5" spans="1:16" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
@@ -2445,10 +2528,10 @@
     </row>
     <row r="6" spans="1:16" ht="20" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
@@ -2475,10 +2558,10 @@
     </row>
     <row r="7" spans="1:16" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C7" s="1">
         <v>6</v>
@@ -2505,10 +2588,10 @@
     </row>
     <row r="8" spans="1:16" ht="20" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -2535,10 +2618,10 @@
     </row>
     <row r="9" spans="1:16" ht="20" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -2567,10 +2650,10 @@
     </row>
     <row r="10" spans="1:16" ht="20" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
@@ -2599,10 +2682,10 @@
     </row>
     <row r="11" spans="1:16" ht="20" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C11" s="1">
         <v>4</v>
@@ -2631,10 +2714,10 @@
     </row>
     <row r="12" spans="1:16" ht="20" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C12" s="1">
         <v>5</v>
@@ -2663,10 +2746,10 @@
     </row>
     <row r="13" spans="1:16" ht="20" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C13" s="1">
         <v>6</v>
@@ -2686,10 +2769,10 @@
     </row>
     <row r="14" spans="1:16" ht="20" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -2709,10 +2792,10 @@
     </row>
     <row r="15" spans="1:16" ht="20" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
@@ -2732,10 +2815,10 @@
     </row>
     <row r="16" spans="1:16" ht="20" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C16" s="1">
         <v>3</v>
@@ -2755,10 +2838,10 @@
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C17" s="1">
         <v>4</v>
@@ -2778,10 +2861,10 @@
     </row>
     <row r="18" spans="1:7" ht="20" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C18" s="1">
         <v>5</v>
@@ -2801,10 +2884,10 @@
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C19" s="1">
         <v>6</v>
@@ -2824,10 +2907,10 @@
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
@@ -2847,10 +2930,10 @@
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1">
       <c r="A21" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
@@ -2870,10 +2953,10 @@
     </row>
     <row r="22" spans="1:7" ht="20" customHeight="1">
       <c r="A22" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C22" s="1">
         <v>3</v>
@@ -2893,10 +2976,10 @@
     </row>
     <row r="23" spans="1:7" ht="20" customHeight="1">
       <c r="A23" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C23" s="1">
         <v>4</v>
@@ -2916,10 +2999,10 @@
     </row>
     <row r="24" spans="1:7" ht="20" customHeight="1">
       <c r="A24" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C24" s="1">
         <v>5</v>
@@ -2939,10 +3022,10 @@
     </row>
     <row r="25" spans="1:7" ht="20" customHeight="1">
       <c r="A25" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C25" s="1">
         <v>6</v>
@@ -2962,10 +3045,10 @@
     </row>
     <row r="26" spans="1:7" ht="20" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -2985,10 +3068,10 @@
     </row>
     <row r="27" spans="1:7" ht="20" customHeight="1">
       <c r="A27" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C27" s="1">
         <v>2</v>
@@ -3008,10 +3091,10 @@
     </row>
     <row r="28" spans="1:7" ht="20" customHeight="1">
       <c r="A28" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C28" s="1">
         <v>3</v>
@@ -3031,10 +3114,10 @@
     </row>
     <row r="29" spans="1:7" ht="20" customHeight="1">
       <c r="A29" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C29" s="1">
         <v>4</v>
@@ -3054,10 +3137,10 @@
     </row>
     <row r="30" spans="1:7" ht="20" customHeight="1">
       <c r="A30" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C30" s="1">
         <v>5</v>
@@ -3077,10 +3160,10 @@
     </row>
     <row r="31" spans="1:7" ht="20" customHeight="1">
       <c r="A31" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C31" s="1">
         <v>6</v>
@@ -3100,10 +3183,10 @@
     </row>
     <row r="32" spans="1:7" ht="20" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
@@ -3123,10 +3206,10 @@
     </row>
     <row r="33" spans="1:7" ht="20" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C33" s="1">
         <v>2</v>
@@ -3146,10 +3229,10 @@
     </row>
     <row r="34" spans="1:7" ht="20" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C34" s="1">
         <v>3</v>
@@ -3169,10 +3252,10 @@
     </row>
     <row r="35" spans="1:7" ht="20" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C35" s="1">
         <v>4</v>
@@ -3192,10 +3275,10 @@
     </row>
     <row r="36" spans="1:7" ht="20" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C36" s="1">
         <v>5</v>
@@ -3215,10 +3298,10 @@
     </row>
     <row r="37" spans="1:7" ht="20" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C37" s="1">
         <v>6</v>
@@ -3248,7 +3331,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -3263,16 +3346,16 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B2" s="1">
         <v>5</v>
@@ -3280,7 +3363,7 @@
     </row>
     <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B3" s="2">
         <v>5</v>
@@ -3288,7 +3371,7 @@
     </row>
     <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B4" s="2">
         <v>5</v>
@@ -3296,7 +3379,7 @@
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B5" s="1">
         <v>5</v>
@@ -3304,7 +3387,7 @@
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B6" s="1">
         <v>15</v>
@@ -3312,7 +3395,7 @@
     </row>
     <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B7" s="1">
         <v>15</v>

</xml_diff>

<commit_message>
finish dev of activateAllianceShrineStage
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -647,7 +647,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="182">
+  <cellStyleXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -662,6 +662,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -871,7 +875,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="182">
+  <cellStyles count="186">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -965,6 +969,8 @@
     <cellStyle name="超链接" xfId="176" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="178" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="184" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -1051,6 +1057,8 @@
     <cellStyle name="访问过的超链接" xfId="177" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="179" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="185" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -1503,7 +1511,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1555,6 +1563,9 @@
     <row r="6" spans="1:6" ht="20" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>108</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dev of alliance fight
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="3100" windowWidth="27520" windowHeight="14540" tabRatio="883" activeTab="5"/>
+    <workbookView xWindow="4420" yWindow="3100" windowWidth="27520" windowHeight="14540" tabRatio="883" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="113">
   <si>
     <t>true</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -485,6 +485,10 @@
   </si>
   <si>
     <t>createAlliance</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_findAllianceToFight</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -647,7 +651,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="186">
+  <cellStyleXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -662,6 +666,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -875,7 +881,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="186">
+  <cellStyles count="188">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -971,6 +977,7 @@
     <cellStyle name="超链接" xfId="180" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="182" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="186" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -1059,6 +1066,7 @@
     <cellStyle name="访问过的超链接" xfId="181" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="183" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="187" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -1622,10 +1630,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:R7"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2:S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1637,7 +1645,7 @@
     <col min="14" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:19" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -1692,8 +1700,11 @@
       <c r="R1" s="3" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="20" customHeight="1">
+      <c r="S1" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1748,8 +1759,11 @@
       <c r="R2" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="20" customHeight="1">
+      <c r="S2" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1804,8 +1818,11 @@
       <c r="R3" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="20" customHeight="1">
+      <c r="S3" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1860,8 +1877,11 @@
       <c r="R4" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="20" customHeight="1">
+      <c r="S4" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1916,8 +1936,11 @@
       <c r="R5" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" ht="20" customHeight="1">
+      <c r="S5" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="20" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1972,8 +1995,11 @@
       <c r="R6" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" ht="20" customHeight="1">
+      <c r="S6" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -2028,8 +2054,11 @@
       <c r="R7" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" ht="20" customHeight="1">
+      <c r="S7" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="20" customHeight="1">
       <c r="M8" s="7"/>
     </row>
   </sheetData>
@@ -3346,7 +3375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
bugfix for alliance shrine event
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="3100" windowWidth="27520" windowHeight="14540" tabRatio="883" activeTab="2"/>
+    <workbookView xWindow="4420" yWindow="3100" windowWidth="27520" windowHeight="14540" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -1518,7 +1518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1573,7 +1573,7 @@
         <v>108</v>
       </c>
       <c r="B6" s="1">
-        <v>3600</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -1632,7 +1632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="S2" sqref="S2:S7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
bugfix for alliance fight
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="4840" windowWidth="27520" windowHeight="14540" tabRatio="883"/>
+    <workbookView xWindow="4760" yWindow="2920" windowWidth="27520" windowHeight="14540" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -1782,7 +1782,7 @@
         <v>110</v>
       </c>
       <c r="B7" s="1">
-        <v>120</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="20" customHeight="1">

</xml_diff>

<commit_message>
dev of alliance help defence
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="460" windowWidth="27520" windowHeight="18140" tabRatio="883"/>
+    <workbookView xWindow="4700" yWindow="1620" windowWidth="27520" windowHeight="18140" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="117">
   <si>
     <t>true</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -501,6 +501,10 @@
   </si>
   <si>
     <t>createAllianceGem</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>allianceHelpDefenceTroopsMaxCount</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -1716,10 +1720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1799,6 +1803,14 @@
       </c>
       <c r="B9" s="1">
         <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="20" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dev of strike player city
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5480" yWindow="1800" windowWidth="27520" windowHeight="18140" tabRatio="883"/>
+    <workbookView xWindow="4200" yWindow="1360" windowWidth="27520" windowHeight="18140" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="118">
   <si>
     <t>true</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -505,6 +505,10 @@
   </si>
   <si>
     <t>allianceHelpDefenceTroopsMaxCount</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>strikeDragonHpDecreasedHpPercent</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -1720,10 +1724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1811,6 +1815,14 @@
       </c>
       <c r="B10" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="20" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="1">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bugfix for alliance fight report
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5480" yWindow="1800" windowWidth="27520" windowHeight="18140" tabRatio="883"/>
+    <workbookView xWindow="4640" yWindow="2100" windowWidth="27520" windowHeight="18140" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="118">
   <si>
     <t>true</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -506,6 +506,9 @@
   <si>
     <t>allianceHelpDefenceTroopsMaxCount</t>
     <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>allianceRevengeMaxTime</t>
   </si>
 </sst>
 </file>
@@ -1720,10 +1723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1811,6 +1814,14 @@
       </c>
       <c r="B10" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="20" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="1">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bugfix for alliance revengeAlliance
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4640" yWindow="2100" windowWidth="27520" windowHeight="18140" tabRatio="883"/>
+    <workbookView xWindow="5340" yWindow="1180" windowWidth="27520" windowHeight="18140" tabRatio="883" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="119">
   <si>
     <t>true</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -509,6 +509,10 @@
   </si>
   <si>
     <t>allianceRevengeMaxTime</t>
+  </si>
+  <si>
+    <t>BOOL_revengeAlliance</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -670,7 +674,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="282">
+  <cellStyleXfs count="284">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -685,6 +689,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -994,7 +1000,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="282">
+  <cellStyles count="284">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -1138,6 +1144,7 @@
     <cellStyle name="超链接" xfId="276" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="278" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="280" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="282" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -1274,6 +1281,7 @@
     <cellStyle name="访问过的超链接" xfId="277" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="279" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="281" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="283" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -1725,8 +1733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1878,10 +1886,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1893,7 +1901,7 @@
     <col min="14" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:20" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -1951,8 +1959,11 @@
       <c r="S1" s="3" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" ht="20" customHeight="1">
+      <c r="T1" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2010,8 +2021,11 @@
       <c r="S2" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" ht="20" customHeight="1">
+      <c r="T2" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2069,8 +2083,11 @@
       <c r="S3" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" ht="20" customHeight="1">
+      <c r="T3" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2128,8 +2145,11 @@
       <c r="S4" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" ht="20" customHeight="1">
+      <c r="T4" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -2187,8 +2207,11 @@
       <c r="S5" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" ht="20" customHeight="1">
+      <c r="T5" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="20" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -2246,8 +2269,11 @@
       <c r="S6" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" ht="20" customHeight="1">
+      <c r="T6" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -2305,8 +2331,11 @@
       <c r="S7" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" ht="20" customHeight="1">
+      <c r="T7" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="20" customHeight="1">
       <c r="M8" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish dev of dragon strike
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4720" yWindow="400" windowWidth="27520" windowHeight="18140" tabRatio="883"/>
+    <workbookView xWindow="4700" yWindow="560" windowWidth="27520" windowHeight="18140" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="120">
   <si>
     <t>true</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -512,6 +512,10 @@
   </si>
   <si>
     <t>BOOL_revengeAlliance</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>dragonStrikeHpDecreasedPercent</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -674,7 +678,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="284">
+  <cellStyleXfs count="288">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -689,6 +693,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1000,7 +1008,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="284">
+  <cellStyles count="288">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -1145,6 +1153,8 @@
     <cellStyle name="超链接" xfId="278" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="280" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="282" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="284" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="286" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -1282,6 +1292,8 @@
     <cellStyle name="访问过的超链接" xfId="279" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="281" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="283" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="285" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="287" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -1731,10 +1743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1830,6 +1842,14 @@
       </c>
       <c r="B11" s="1">
         <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="20" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dev of attack player city
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -1746,7 +1746,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1809,7 +1809,7 @@
         <v>110</v>
       </c>
       <c r="B7" s="1">
-        <v>60</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="20" customHeight="1">
@@ -1825,7 +1825,7 @@
         <v>109</v>
       </c>
       <c r="B9" s="1">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20" customHeight="1">

</xml_diff>

<commit_message>
finish dev of attack player city
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5680" yWindow="320" windowWidth="27520" windowHeight="18140" tabRatio="883"/>
+    <workbookView xWindow="5320" yWindow="1520" windowWidth="27520" windowHeight="18140" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -1809,7 +1809,7 @@
         <v>110</v>
       </c>
       <c r="B7" s="1">
-        <v>12</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="20" customHeight="1">
@@ -1825,7 +1825,7 @@
         <v>109</v>
       </c>
       <c r="B9" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20" customHeight="1">

</xml_diff>

<commit_message>
dev of attack alliance shrine stage
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="1520" windowWidth="27520" windowHeight="18140" tabRatio="883"/>
+    <workbookView xWindow="5340" yWindow="1080" windowWidth="27520" windowHeight="18140" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="122">
   <si>
     <t>true</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -476,10 +476,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>allianceFightTimePerFight</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>allianceFightPrepareTime</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -516,6 +512,18 @@
   </si>
   <si>
     <t>dragonStrikeHpDecreasedPercent</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>allianceRegionMapBaseTimePerGrid</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>allianceRegionMapWidth</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>allianceRegionMapHeight</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -678,7 +686,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="288">
+  <cellStyleXfs count="292">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -693,6 +701,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1008,7 +1020,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="288">
+  <cellStyles count="292">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -1155,6 +1167,8 @@
     <cellStyle name="超链接" xfId="282" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="284" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="286" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="288" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="290" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -1294,6 +1308,8 @@
     <cellStyle name="访问过的超链接" xfId="283" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="285" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="287" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="289" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="291" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -1743,7 +1759,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -1766,7 +1782,7 @@
     </row>
     <row r="2" spans="1:6" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" s="1">
         <v>50</v>
@@ -1774,7 +1790,7 @@
     </row>
     <row r="3" spans="1:6" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" s="2">
         <v>100</v>
@@ -1782,7 +1798,7 @@
     </row>
     <row r="4" spans="1:6" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B4" s="2">
         <v>50</v>
@@ -1790,7 +1806,7 @@
     </row>
     <row r="5" spans="1:6" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B5" s="1">
         <v>50</v>
@@ -1798,15 +1814,15 @@
     </row>
     <row r="6" spans="1:6" ht="20" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="1">
-        <v>60</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" s="1">
         <v>60</v>
@@ -1822,10 +1838,10 @@
     </row>
     <row r="9" spans="1:6" ht="20" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B9" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20" customHeight="1">
@@ -1833,15 +1849,15 @@
         <v>116</v>
       </c>
       <c r="B10" s="1">
-        <v>2</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B11" s="1">
-        <v>300</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="20" customHeight="1">
@@ -1849,7 +1865,23 @@
         <v>119</v>
       </c>
       <c r="B12" s="1">
-        <v>5</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="20" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="20" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="1">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1980,7 +2012,7 @@
         <v>107</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="20" customHeight="1">

</xml_diff>

<commit_message>
finish dev of strike player city
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="1700" windowWidth="27520" windowHeight="18140" tabRatio="883"/>
+    <workbookView xWindow="6680" yWindow="640" windowWidth="27520" windowHeight="18140" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="121">
   <si>
     <t>true</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -508,10 +508,6 @@
   </si>
   <si>
     <t>BOOL_revengeAlliance</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>dragonStrikeHpDecreasedPercent</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
@@ -686,7 +682,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="292">
+  <cellStyleXfs count="296">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -701,6 +697,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1020,7 +1020,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="292">
+  <cellStyles count="296">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -1169,6 +1169,8 @@
     <cellStyle name="超链接" xfId="286" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="288" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="290" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="292" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="294" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -1310,6 +1312,8 @@
     <cellStyle name="访问过的超链接" xfId="287" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="289" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="291" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="293" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="295" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -1759,10 +1763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1825,7 +1829,7 @@
         <v>109</v>
       </c>
       <c r="B7" s="1">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="20" customHeight="1">
@@ -1833,7 +1837,7 @@
         <v>108</v>
       </c>
       <c r="B8" s="1">
-        <v>15</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="20" customHeight="1">
@@ -1857,7 +1861,7 @@
         <v>118</v>
       </c>
       <c r="B11" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="20" customHeight="1">
@@ -1865,7 +1869,7 @@
         <v>119</v>
       </c>
       <c r="B12" s="1">
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="20" customHeight="1">
@@ -1873,14 +1877,6 @@
         <v>120</v>
       </c>
       <c r="B13" s="1">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1">
-      <c r="A14" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14" s="1">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
bugfix for strike player city
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="6680" yWindow="640" windowWidth="27520" windowHeight="18140" tabRatio="883"/>
@@ -1766,7 +1766,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
finish dev of dragon leadership
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -1809,7 +1809,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1872,7 +1872,7 @@
         <v>109</v>
       </c>
       <c r="B7" s="1">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="20" customHeight="1">
@@ -1880,7 +1880,7 @@
         <v>108</v>
       </c>
       <c r="B8" s="1">
-        <v>30</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="20" customHeight="1">

</xml_diff>

<commit_message>
dev of attack alliance village
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -1809,7 +1809,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1872,7 +1872,7 @@
         <v>109</v>
       </c>
       <c r="B7" s="1">
-        <v>5</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="20" customHeight="1">
@@ -1880,7 +1880,7 @@
         <v>108</v>
       </c>
       <c r="B8" s="1">
-        <v>30</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="20" customHeight="1">

</xml_diff>

<commit_message>
bugfix for attack player city
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="1040" windowWidth="22760" windowHeight="15040" tabRatio="883"/>
+    <workbookView xWindow="7460" yWindow="3360" windowWidth="22760" windowHeight="15040" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -1809,7 +1809,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1864,7 +1864,7 @@
         <v>110</v>
       </c>
       <c r="B6" s="1">
-        <v>7</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="20" customHeight="1">

</xml_diff>

<commit_message>
finish dev of collect resource exp add
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7600" yWindow="4480" windowWidth="22760" windowHeight="15040" tabRatio="883"/>
+    <workbookView xWindow="6720" yWindow="2560" windowWidth="22760" windowHeight="15040" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="131">
   <si>
     <t>true</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -548,7 +548,23 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>collectedResourceCountPerExp</t>
+    <t>collectedWoodCountPerExp</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>collectedStoneCountPerExp</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>collectedIronCountPerExp</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>collectedFoodCountPerExp</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>collectedCoinCountPerExp</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -712,7 +728,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="300">
+  <cellStyleXfs count="302">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -727,6 +743,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1063,7 +1081,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="300">
+  <cellStyles count="302">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -1216,6 +1234,7 @@
     <cellStyle name="超链接" xfId="294" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="296" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="298" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="300" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -1361,6 +1380,7 @@
     <cellStyle name="访问过的超链接" xfId="295" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="297" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="299" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="301" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -1810,10 +1830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1940,6 +1960,38 @@
         <v>126</v>
       </c>
       <c r="B15" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="20" customHeight="1">
+      <c r="A16" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="20" customHeight="1">
+      <c r="A17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="20" customHeight="1">
+      <c r="A18" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="20" customHeight="1">
+      <c r="A19" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="1">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dev of alliance fight status changed
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="2560" windowWidth="22760" windowHeight="15040" tabRatio="883"/>
+    <workbookView xWindow="6440" yWindow="2760" windowWidth="22760" windowHeight="15040" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -1833,7 +1833,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1896,7 +1896,7 @@
         <v>109</v>
       </c>
       <c r="B7" s="1">
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="20" customHeight="1">
@@ -1904,7 +1904,7 @@
         <v>108</v>
       </c>
       <c r="B8" s="1">
-        <v>300</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="20" customHeight="1">

</xml_diff>

<commit_message>
finish dev of alliance status changed
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6440" yWindow="2760" windowWidth="22760" windowHeight="15040" tabRatio="883"/>
+    <workbookView xWindow="8380" yWindow="2600" windowWidth="22760" windowHeight="15040" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -1896,7 +1896,7 @@
         <v>109</v>
       </c>
       <c r="B7" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="20" customHeight="1">
@@ -1904,7 +1904,7 @@
         <v>108</v>
       </c>
       <c r="B8" s="1">
-        <v>12</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="20" customHeight="1">

</xml_diff>

<commit_message>
dev of recover server data
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="2140" windowWidth="22760" windowHeight="15040" tabRatio="883"/>
+    <workbookView xWindow="8060" yWindow="3140" windowWidth="22760" windowHeight="15040" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -1833,7 +1833,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
bugfix for hatch dragon
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9520" yWindow="3840" windowWidth="22760" windowHeight="15040" tabRatio="883"/>
+    <workbookView xWindow="7600" yWindow="3560" windowWidth="22760" windowHeight="15040" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="132">
   <si>
     <t>true</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -565,6 +565,10 @@
   </si>
   <si>
     <t>collectedCoinCountPerExp</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>playerHatchDragonNeedHours</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -1830,10 +1834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1993,6 +1997,14 @@
       </c>
       <c r="B19" s="1">
         <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="20" customHeight="1">
+      <c r="A20" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B20" s="1">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish dev of alliance shop
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -584,7 +584,7 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>BOOL_buyItem</t>
+    <t>BOOL_addItem</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -2156,7 +2156,7 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2:U7"/>
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
dev of give loyalty to alliance member
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9280" yWindow="4080" windowWidth="22760" windowHeight="15040" tabRatio="883"/>
+    <workbookView xWindow="2580" yWindow="40" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="141">
   <si>
     <t>true</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -585,6 +585,26 @@
   </si>
   <si>
     <t>killScorePerWallHp</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_giveLoyaltyToAllianceMember</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>false</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>false</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -1868,7 +1888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -2153,10 +2173,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2165,10 +2185,12 @@
     <col min="3" max="5" width="20.6640625" style="6"/>
     <col min="6" max="12" width="20.6640625" style="1"/>
     <col min="13" max="13" width="20.6640625" style="6"/>
-    <col min="14" max="16384" width="20.6640625" style="1"/>
+    <col min="14" max="21" width="20.6640625" style="1"/>
+    <col min="22" max="22" width="20.6640625" style="6"/>
+    <col min="23" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:22" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -2232,8 +2254,11 @@
       <c r="U1" s="3" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" ht="20" customHeight="1">
+      <c r="V1" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2297,8 +2322,11 @@
       <c r="U2" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" ht="20" customHeight="1">
+      <c r="V2" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2362,8 +2390,11 @@
       <c r="U3" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" ht="20" customHeight="1">
+      <c r="V3" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2427,8 +2458,11 @@
       <c r="U4" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" ht="20" customHeight="1">
+      <c r="V4" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -2492,8 +2526,11 @@
       <c r="U5" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" ht="20" customHeight="1">
+      <c r="V5" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="20" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -2557,8 +2594,11 @@
       <c r="U6" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" ht="20" customHeight="1">
+      <c r="V6" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -2622,8 +2662,11 @@
       <c r="U7" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" ht="20" customHeight="1">
+      <c r="V7" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="20" customHeight="1">
       <c r="M8" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dev of dragons buff
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="40" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="3"/>
+    <workbookView xWindow="7300" yWindow="2620" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -1888,8 +1888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2175,7 +2175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="Q1" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
dev of buff effect
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -1889,7 +1889,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1944,7 +1944,7 @@
         <v>110</v>
       </c>
       <c r="B6" s="1">
-        <v>120</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="20" customHeight="1">

</xml_diff>

<commit_message>
finish dev of item buff
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7300" yWindow="2620" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
+    <workbookView xWindow="15840" yWindow="2860" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="140">
   <si>
     <t>true</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -513,10 +513,6 @@
   </si>
   <si>
     <t>BOOL_revengeAlliance</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>allianceRegionMapBaseTimePerGrid</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
@@ -1886,10 +1882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1944,7 +1940,7 @@
         <v>110</v>
       </c>
       <c r="B6" s="1">
-        <v>7</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="20" customHeight="1">
@@ -1984,7 +1980,7 @@
         <v>118</v>
       </c>
       <c r="B11" s="1">
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="20" customHeight="1">
@@ -1997,10 +1993,10 @@
     </row>
     <row r="13" spans="1:6" ht="20" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B13" s="1">
-        <v>51</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="20" customHeight="1">
@@ -2008,7 +2004,7 @@
         <v>124</v>
       </c>
       <c r="B14" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="20" customHeight="1">
@@ -2040,14 +2036,6 @@
         <v>128</v>
       </c>
       <c r="B18" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="20" customHeight="1">
-      <c r="A19" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B19" s="1">
         <v>50</v>
       </c>
     </row>
@@ -2083,13 +2071,13 @@
         <v>18</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" s="13">
         <v>0.5</v>
@@ -2097,7 +2085,7 @@
     </row>
     <row r="3" spans="1:6" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="14">
         <v>0.5</v>
@@ -2105,7 +2093,7 @@
     </row>
     <row r="4" spans="1:6" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B4" s="13">
         <v>1</v>
@@ -2113,7 +2101,7 @@
     </row>
     <row r="5" spans="1:6" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B5" s="13">
         <v>0.1</v>
@@ -2252,10 +2240,10 @@
         <v>117</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="20" customHeight="1">
@@ -2287,7 +2275,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>0</v>
@@ -2323,7 +2311,7 @@
         <v>0</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="20" customHeight="1">
@@ -2340,7 +2328,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>0</v>
@@ -2352,46 +2340,46 @@
         <v>1</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="V3" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="20" customHeight="1">
@@ -2408,7 +2396,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>0</v>
@@ -2420,31 +2408,31 @@
         <v>1</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="R4" s="7" t="s">
         <v>1</v>
@@ -2459,7 +2447,7 @@
         <v>0</v>
       </c>
       <c r="V4" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="20" customHeight="1">
@@ -2482,22 +2470,22 @@
         <v>0</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M5" s="7" t="s">
         <v>80</v>
@@ -2527,7 +2515,7 @@
         <v>1</v>
       </c>
       <c r="V5" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="20" customHeight="1">
@@ -2595,7 +2583,7 @@
         <v>1</v>
       </c>
       <c r="V6" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="20" customHeight="1">
@@ -2663,7 +2651,7 @@
         <v>1</v>
       </c>
       <c r="V7" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="20" customHeight="1">

</xml_diff>

<commit_message>
finish dev of production tech buff efffect
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15840" yWindow="2860" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
+    <workbookView xWindow="4240" yWindow="1880" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
finish dev of vip effects
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6080" yWindow="2000" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
+    <workbookView xWindow="12260" yWindow="2380" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="142">
   <si>
     <t>true</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -605,6 +605,10 @@
   </si>
   <si>
     <t>dragonStrikeHpDecreasedPercent</t>
+  </si>
+  <si>
+    <t>allianceFightFaiedProtectMinutes</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -767,7 +771,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="310">
+  <cellStyleXfs count="314">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -782,6 +786,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1128,7 +1136,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="310">
+  <cellStyles count="314">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -1286,6 +1294,8 @@
     <cellStyle name="超链接" xfId="304" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="306" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="308" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="310" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="312" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -1436,6 +1446,8 @@
     <cellStyle name="访问过的超链接" xfId="305" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="307" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="309" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="311" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="313" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -1885,10 +1897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2048,6 +2060,14 @@
       </c>
       <c r="B19" s="1">
         <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="20" customHeight="1">
+      <c r="A20" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2066,8 +2086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
dev of account system
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12260" yWindow="2380" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="1"/>
+    <workbookView xWindow="7540" yWindow="1860" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="143">
   <si>
     <t>true</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -111,10 +111,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>BOOL_handleJoinAllianceRequest</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>BOOL_editAllianceJoinType</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -608,6 +604,14 @@
   </si>
   <si>
     <t>allianceFightFaiedProtectMinutes</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_approveJoinAllianceRequest</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL_removeJoinAllianceReqeusts</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -771,7 +775,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="314">
+  <cellStyleXfs count="316">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -786,6 +790,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1136,7 +1142,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="314">
+  <cellStyles count="316">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -1296,6 +1302,7 @@
     <cellStyle name="超链接" xfId="308" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="310" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="312" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="314" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -1448,6 +1455,7 @@
     <cellStyle name="访问过的超链接" xfId="309" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="311" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="313" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="315" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -1911,16 +1919,16 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" s="1">
         <v>50</v>
@@ -1928,7 +1936,7 @@
     </row>
     <row r="3" spans="1:6" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" s="2">
         <v>100</v>
@@ -1936,7 +1944,7 @@
     </row>
     <row r="4" spans="1:6" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="2">
         <v>50</v>
@@ -1944,7 +1952,7 @@
     </row>
     <row r="5" spans="1:6" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="1">
         <v>50</v>
@@ -1952,7 +1960,7 @@
     </row>
     <row r="6" spans="1:6" ht="20" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" s="1">
         <v>120</v>
@@ -1960,7 +1968,7 @@
     </row>
     <row r="7" spans="1:6" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
@@ -1968,7 +1976,7 @@
     </row>
     <row r="8" spans="1:6" ht="20" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B8" s="1">
         <v>300</v>
@@ -1976,7 +1984,7 @@
     </row>
     <row r="9" spans="1:6" ht="20" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
@@ -1984,7 +1992,7 @@
     </row>
     <row r="10" spans="1:6" ht="20" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B10" s="1">
         <v>300</v>
@@ -1992,7 +2000,7 @@
     </row>
     <row r="11" spans="1:6" ht="20" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B11" s="1">
         <v>51</v>
@@ -2000,7 +2008,7 @@
     </row>
     <row r="12" spans="1:6" ht="20" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B12" s="1">
         <v>51</v>
@@ -2008,7 +2016,7 @@
     </row>
     <row r="13" spans="1:6" ht="20" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B13" s="1">
         <v>100</v>
@@ -2016,7 +2024,7 @@
     </row>
     <row r="14" spans="1:6" ht="20" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B14" s="1">
         <v>50</v>
@@ -2024,7 +2032,7 @@
     </row>
     <row r="15" spans="1:6" ht="20" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B15" s="1">
         <v>50</v>
@@ -2032,7 +2040,7 @@
     </row>
     <row r="16" spans="1:6" ht="20" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B16" s="1">
         <v>50</v>
@@ -2040,7 +2048,7 @@
     </row>
     <row r="17" spans="1:2" ht="20" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B17" s="1">
         <v>50</v>
@@ -2048,7 +2056,7 @@
     </row>
     <row r="18" spans="1:2" ht="20" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B18" s="1">
         <v>50</v>
@@ -2056,7 +2064,7 @@
     </row>
     <row r="19" spans="1:2" ht="20" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B19" s="1">
         <v>10</v>
@@ -2064,7 +2072,7 @@
     </row>
     <row r="20" spans="1:2" ht="20" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B20" s="1">
         <v>2</v>
@@ -2086,7 +2094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2099,16 +2107,16 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B2" s="13">
         <v>0.5</v>
@@ -2116,7 +2124,7 @@
     </row>
     <row r="3" spans="1:6" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B3" s="14">
         <v>0.5</v>
@@ -2124,7 +2132,7 @@
     </row>
     <row r="4" spans="1:6" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B4" s="13">
         <v>1</v>
@@ -2132,7 +2140,7 @@
     </row>
     <row r="5" spans="1:6" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B5" s="13">
         <v>0.1</v>
@@ -2165,10 +2173,10 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F1" s="4"/>
     </row>
@@ -2192,24 +2200,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V8"/>
+  <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="20.6640625" style="1"/>
     <col min="3" max="5" width="20.6640625" style="6"/>
-    <col min="6" max="12" width="20.6640625" style="1"/>
-    <col min="13" max="13" width="20.6640625" style="6"/>
-    <col min="14" max="21" width="20.6640625" style="1"/>
-    <col min="22" max="22" width="20.6640625" style="6"/>
-    <col min="23" max="16384" width="20.6640625" style="1"/>
+    <col min="6" max="13" width="20.6640625" style="1"/>
+    <col min="14" max="14" width="20.6640625" style="6"/>
+    <col min="15" max="22" width="20.6640625" style="1"/>
+    <col min="23" max="23" width="20.6640625" style="6"/>
+    <col min="24" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:23" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -2217,7 +2225,7 @@
         <v>9</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>10</v>
@@ -2229,10 +2237,10 @@
         <v>12</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>13</v>
@@ -2241,43 +2249,46 @@
         <v>14</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>15</v>
+        <v>141</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>104</v>
-      </c>
       <c r="S1" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" ht="20" customHeight="1">
+        <v>116</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2306,7 +2317,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>0</v>
@@ -2342,10 +2353,13 @@
         <v>0</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="20" customHeight="1">
+        <v>0</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2359,7 +2373,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>0</v>
@@ -2371,49 +2385,52 @@
         <v>1</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>131</v>
+        <v>0</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>1</v>
+        <v>130</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="U3" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="V3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="V3" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="20" customHeight="1">
+      <c r="W3" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2427,7 +2444,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>0</v>
@@ -2439,34 +2456,34 @@
         <v>1</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>131</v>
+        <v>0</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>1</v>
+        <v>130</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>1</v>
+        <v>130</v>
       </c>
       <c r="S4" s="7" t="s">
         <v>1</v>
@@ -2475,13 +2492,16 @@
         <v>1</v>
       </c>
       <c r="U4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="V4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="V4" s="6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="20" customHeight="1">
+      <c r="W4" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -2501,31 +2521,31 @@
         <v>0</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>131</v>
+        <v>0</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="P5" s="7" t="s">
         <v>1</v>
@@ -2545,11 +2565,14 @@
       <c r="U5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="V5" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="20" customHeight="1">
+      <c r="V5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="W5" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="20" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -2613,11 +2636,14 @@
       <c r="U6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="V6" s="6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="20" customHeight="1">
+      <c r="V6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -2681,12 +2707,15 @@
       <c r="U7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="V7" s="6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="20" customHeight="1">
-      <c r="M8" s="7"/>
+      <c r="V7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="20" customHeight="1">
+      <c r="N8" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -2719,24 +2748,24 @@
   <sheetData>
     <row r="1" spans="1:13" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1">
         <v>3</v>
@@ -2745,7 +2774,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E2" s="8">
         <v>120</v>
@@ -2760,7 +2789,7 @@
     </row>
     <row r="3" spans="1:13" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -2769,7 +2798,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3" s="8">
         <v>80</v>
@@ -2784,7 +2813,7 @@
     </row>
     <row r="4" spans="1:13" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -2793,7 +2822,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="8">
         <v>40</v>
@@ -2808,7 +2837,7 @@
     </row>
     <row r="5" spans="1:13" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -2817,7 +2846,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5" s="8">
         <v>20</v>
@@ -2832,7 +2861,7 @@
     </row>
     <row r="6" spans="1:13" ht="20" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -2841,7 +2870,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E6" s="8">
         <v>20</v>
@@ -2856,7 +2885,7 @@
     </row>
     <row r="7" spans="1:13" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -2865,7 +2894,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E7" s="8">
         <v>20</v>
@@ -2880,7 +2909,7 @@
     </row>
     <row r="8" spans="1:13" ht="20" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1">
         <v>3</v>
@@ -2889,7 +2918,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="9">
         <v>0</v>
@@ -2905,7 +2934,7 @@
     </row>
     <row r="9" spans="1:13" ht="20" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -2914,7 +2943,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="9">
         <v>0</v>
@@ -2930,7 +2959,7 @@
     </row>
     <row r="10" spans="1:13" ht="20" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -2939,7 +2968,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E10" s="9">
         <v>0</v>
@@ -2955,7 +2984,7 @@
     </row>
     <row r="11" spans="1:13" ht="20" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -2964,7 +2993,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E11" s="8">
         <v>0</v>
@@ -2972,7 +3001,7 @@
     </row>
     <row r="12" spans="1:13" ht="20" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -2981,7 +3010,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E12" s="8">
         <v>0</v>
@@ -2989,7 +3018,7 @@
     </row>
     <row r="13" spans="1:13" ht="20" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -2998,7 +3027,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E13" s="8">
         <v>0</v>
@@ -3006,7 +3035,7 @@
     </row>
     <row r="14" spans="1:13" ht="20" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -3015,7 +3044,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E14" s="8">
         <v>0</v>
@@ -3051,34 +3080,34 @@
   <sheetData>
     <row r="1" spans="1:16" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="E1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:16" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -3105,10 +3134,10 @@
     </row>
     <row r="3" spans="1:16" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -3135,10 +3164,10 @@
     </row>
     <row r="4" spans="1:16" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
@@ -3165,10 +3194,10 @@
     </row>
     <row r="5" spans="1:16" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
@@ -3195,10 +3224,10 @@
     </row>
     <row r="6" spans="1:16" ht="20" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
@@ -3225,10 +3254,10 @@
     </row>
     <row r="7" spans="1:16" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="1">
         <v>6</v>
@@ -3255,10 +3284,10 @@
     </row>
     <row r="8" spans="1:16" ht="20" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -3285,10 +3314,10 @@
     </row>
     <row r="9" spans="1:16" ht="20" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -3317,10 +3346,10 @@
     </row>
     <row r="10" spans="1:16" ht="20" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
@@ -3349,10 +3378,10 @@
     </row>
     <row r="11" spans="1:16" ht="20" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" s="1">
         <v>4</v>
@@ -3381,10 +3410,10 @@
     </row>
     <row r="12" spans="1:16" ht="20" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" s="1">
         <v>5</v>
@@ -3413,10 +3442,10 @@
     </row>
     <row r="13" spans="1:16" ht="20" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" s="1">
         <v>6</v>
@@ -3436,10 +3465,10 @@
     </row>
     <row r="14" spans="1:16" ht="20" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -3459,10 +3488,10 @@
     </row>
     <row r="15" spans="1:16" ht="20" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
@@ -3482,10 +3511,10 @@
     </row>
     <row r="16" spans="1:16" ht="20" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" s="1">
         <v>3</v>
@@ -3505,10 +3534,10 @@
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C17" s="1">
         <v>4</v>
@@ -3528,10 +3557,10 @@
     </row>
     <row r="18" spans="1:7" ht="20" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" s="1">
         <v>5</v>
@@ -3551,10 +3580,10 @@
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C19" s="1">
         <v>6</v>
@@ -3574,10 +3603,10 @@
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
@@ -3597,10 +3626,10 @@
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1">
       <c r="A21" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
@@ -3620,10 +3649,10 @@
     </row>
     <row r="22" spans="1:7" ht="20" customHeight="1">
       <c r="A22" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" s="1">
         <v>3</v>
@@ -3643,10 +3672,10 @@
     </row>
     <row r="23" spans="1:7" ht="20" customHeight="1">
       <c r="A23" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C23" s="1">
         <v>4</v>
@@ -3666,10 +3695,10 @@
     </row>
     <row r="24" spans="1:7" ht="20" customHeight="1">
       <c r="A24" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C24" s="1">
         <v>5</v>
@@ -3689,10 +3718,10 @@
     </row>
     <row r="25" spans="1:7" ht="20" customHeight="1">
       <c r="A25" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C25" s="1">
         <v>6</v>
@@ -3712,10 +3741,10 @@
     </row>
     <row r="26" spans="1:7" ht="20" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -3735,10 +3764,10 @@
     </row>
     <row r="27" spans="1:7" ht="20" customHeight="1">
       <c r="A27" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C27" s="1">
         <v>2</v>
@@ -3758,10 +3787,10 @@
     </row>
     <row r="28" spans="1:7" ht="20" customHeight="1">
       <c r="A28" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C28" s="1">
         <v>3</v>
@@ -3781,10 +3810,10 @@
     </row>
     <row r="29" spans="1:7" ht="20" customHeight="1">
       <c r="A29" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C29" s="1">
         <v>4</v>
@@ -3804,10 +3833,10 @@
     </row>
     <row r="30" spans="1:7" ht="20" customHeight="1">
       <c r="A30" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C30" s="1">
         <v>5</v>
@@ -3827,10 +3856,10 @@
     </row>
     <row r="31" spans="1:7" ht="20" customHeight="1">
       <c r="A31" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C31" s="1">
         <v>6</v>
@@ -3850,10 +3879,10 @@
     </row>
     <row r="32" spans="1:7" ht="20" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
@@ -3873,10 +3902,10 @@
     </row>
     <row r="33" spans="1:7" ht="20" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C33" s="1">
         <v>2</v>
@@ -3896,10 +3925,10 @@
     </row>
     <row r="34" spans="1:7" ht="20" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C34" s="1">
         <v>3</v>
@@ -3919,10 +3948,10 @@
     </row>
     <row r="35" spans="1:7" ht="20" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C35" s="1">
         <v>4</v>
@@ -3942,10 +3971,10 @@
     </row>
     <row r="36" spans="1:7" ht="20" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C36" s="1">
         <v>5</v>
@@ -3965,10 +3994,10 @@
     </row>
     <row r="37" spans="1:7" ht="20" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C37" s="1">
         <v>6</v>
@@ -4013,16 +4042,16 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
@@ -4030,7 +4059,7 @@
     </row>
     <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="2">
         <v>5</v>
@@ -4038,7 +4067,7 @@
     </row>
     <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
@@ -4046,7 +4075,7 @@
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" s="1">
         <v>5</v>
@@ -4054,7 +4083,7 @@
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" s="1">
         <v>15</v>
@@ -4062,7 +4091,7 @@
     </row>
     <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" s="1">
         <v>15</v>

</xml_diff>

<commit_message>
finish rebuild of shrine
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceInitData.xlsx
+++ b/gameData/shared/AllianceInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="100" windowWidth="33420" windowHeight="20860" tabRatio="497"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="497" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="566">
   <si>
     <t>true</t>
     <phoneticPr fontId="9" type="noConversion"/>
@@ -660,9 +660,6 @@
   </si>
   <si>
     <t>INT_needPerception</t>
-  </si>
-  <si>
-    <t>INT_suggestPlayer</t>
   </si>
   <si>
     <t>INT_suggestPower</t>
@@ -4436,8 +4433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -4583,13 +4580,13 @@
     </row>
     <row r="13" spans="1:6" ht="20" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B13" s="8">
         <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="20" customHeight="1">
@@ -4660,112 +4657,112 @@
     </row>
     <row r="20" spans="1:3" ht="20" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B20" s="8">
         <v>120</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="20" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B21" s="8">
         <v>240</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="20" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B22" s="8">
         <v>40</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="20" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B23" s="8">
         <v>30</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="20" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B24" s="8">
         <v>20</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="20" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B25" s="8">
         <v>360</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="20" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B26" s="8">
         <v>41</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="20" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B27" s="8">
         <v>20000</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="20" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B28" s="8">
         <v>10</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="20" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B29" s="8">
         <v>10080</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
   </sheetData>
@@ -4868,7 +4865,7 @@
         <v>14</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>46</v>
@@ -4892,7 +4889,7 @@
         <v>32</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>35</v>
@@ -4904,7 +4901,7 @@
         <v>40</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="20" customHeight="1">
@@ -6147,7 +6144,7 @@
     </row>
     <row r="32" spans="1:7" ht="20" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>144</v>
@@ -6170,7 +6167,7 @@
     </row>
     <row r="33" spans="1:7" ht="20" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>144</v>
@@ -6193,7 +6190,7 @@
     </row>
     <row r="34" spans="1:7" ht="20" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>144</v>
@@ -6216,7 +6213,7 @@
     </row>
     <row r="35" spans="1:7" ht="20" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>144</v>
@@ -6239,7 +6236,7 @@
     </row>
     <row r="36" spans="1:7" ht="20" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>144</v>
@@ -6262,7 +6259,7 @@
     </row>
     <row r="37" spans="1:7" ht="20" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>144</v>
@@ -6306,31 +6303,31 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V29"/>
+  <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="5" width="20.6640625" style="12"/>
-    <col min="6" max="7" width="24.1640625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="21.1640625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="91.5" style="12" customWidth="1"/>
-    <col min="10" max="14" width="20.6640625" style="12"/>
-    <col min="15" max="15" width="22.83203125" style="12" customWidth="1"/>
-    <col min="16" max="16" width="34.5" style="12" customWidth="1"/>
-    <col min="17" max="17" width="20.6640625" style="12"/>
-    <col min="18" max="18" width="28" style="12" customWidth="1"/>
-    <col min="19" max="19" width="29.6640625" style="12" customWidth="1"/>
-    <col min="20" max="20" width="20.6640625" style="12"/>
-    <col min="21" max="21" width="32.5" style="12" customWidth="1"/>
-    <col min="22" max="22" width="31.5" style="12" customWidth="1"/>
-    <col min="23" max="16384" width="20.6640625" style="12"/>
+    <col min="6" max="6" width="24.1640625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="91.5" style="12" customWidth="1"/>
+    <col min="9" max="13" width="20.6640625" style="12"/>
+    <col min="14" max="14" width="22.83203125" style="12" customWidth="1"/>
+    <col min="15" max="15" width="34.5" style="12" customWidth="1"/>
+    <col min="16" max="16" width="20.6640625" style="12"/>
+    <col min="17" max="17" width="28" style="12" customWidth="1"/>
+    <col min="18" max="18" width="29.6640625" style="12" customWidth="1"/>
+    <col min="19" max="19" width="20.6640625" style="12"/>
+    <col min="20" max="20" width="32.5" style="12" customWidth="1"/>
+    <col min="21" max="21" width="31.5" style="12" customWidth="1"/>
+    <col min="22" max="16384" width="20.6640625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="13" customFormat="1" ht="30">
+    <row r="1" spans="1:21" s="13" customFormat="1" ht="30">
       <c r="A1" s="14" t="s">
         <v>159</v>
       </c>
@@ -6356,10 +6353,10 @@
         <v>166</v>
       </c>
       <c r="I1" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>167</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>497</v>
       </c>
       <c r="K1" s="14" t="s">
         <v>168</v>
@@ -6394,11 +6391,8 @@
       <c r="U1" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="V1" s="14" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" ht="45">
+    </row>
+    <row r="2" spans="1:21" ht="45">
       <c r="A2" s="15" t="s">
         <v>145</v>
       </c>
@@ -6417,56 +6411,53 @@
       <c r="F2" s="15">
         <v>50</v>
       </c>
-      <c r="G2" s="15">
-        <v>4</v>
-      </c>
-      <c r="H2" s="16">
+      <c r="G2" s="16">
         <v>80</v>
       </c>
-      <c r="I2" s="17" t="s">
-        <v>508</v>
+      <c r="H2" s="17" t="s">
+        <v>507</v>
+      </c>
+      <c r="I2" s="15">
+        <v>200</v>
       </c>
       <c r="J2" s="15">
-        <v>600</v>
+        <v>15</v>
       </c>
       <c r="K2" s="15">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L2" s="15">
-        <v>20</v>
-      </c>
-      <c r="M2" s="15">
         <v>35</v>
       </c>
+      <c r="M2" s="17" t="s">
+        <v>180</v>
+      </c>
       <c r="N2" s="17" t="s">
-        <v>181</v>
+        <v>216</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>217</v>
+        <v>335</v>
       </c>
       <c r="P2" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="R2" s="17" t="s">
         <v>336</v>
       </c>
-      <c r="Q2" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="R2" s="17" t="s">
-        <v>247</v>
-      </c>
       <c r="S2" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="T2" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="U2" s="17" t="s">
         <v>337</v>
       </c>
-      <c r="T2" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="U2" s="17" t="s">
-        <v>232</v>
-      </c>
-      <c r="V2" s="17" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="45">
+    </row>
+    <row r="3" spans="1:21" ht="45">
       <c r="A3" s="15" t="s">
         <v>146</v>
       </c>
@@ -6485,56 +6476,53 @@
       <c r="F3" s="15">
         <v>50</v>
       </c>
-      <c r="G3" s="15">
-        <v>4</v>
-      </c>
-      <c r="H3" s="16">
+      <c r="G3" s="16">
         <v>180</v>
       </c>
-      <c r="I3" s="17" t="s">
-        <v>509</v>
+      <c r="H3" s="17" t="s">
+        <v>508</v>
+      </c>
+      <c r="I3" s="15">
+        <v>400</v>
       </c>
       <c r="J3" s="15">
-        <v>1200</v>
+        <v>30</v>
       </c>
       <c r="K3" s="15">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="L3" s="15">
-        <v>45</v>
-      </c>
-      <c r="M3" s="15">
         <v>75</v>
       </c>
+      <c r="M3" s="17" t="s">
+        <v>181</v>
+      </c>
       <c r="N3" s="17" t="s">
-        <v>182</v>
+        <v>217</v>
       </c>
       <c r="O3" s="17" t="s">
-        <v>218</v>
+        <v>338</v>
       </c>
       <c r="P3" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="R3" s="17" t="s">
         <v>339</v>
       </c>
-      <c r="Q3" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="R3" s="17" t="s">
-        <v>248</v>
-      </c>
       <c r="S3" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="T3" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="U3" s="17" t="s">
         <v>340</v>
       </c>
-      <c r="T3" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="U3" s="17" t="s">
-        <v>233</v>
-      </c>
-      <c r="V3" s="17" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="45">
+    </row>
+    <row r="4" spans="1:21" ht="45">
       <c r="A4" s="15" t="s">
         <v>90</v>
       </c>
@@ -6553,56 +6541,53 @@
       <c r="F4" s="15">
         <v>50</v>
       </c>
-      <c r="G4" s="15">
-        <v>4</v>
-      </c>
-      <c r="H4" s="16">
+      <c r="G4" s="16">
         <v>280</v>
       </c>
-      <c r="I4" s="17" t="s">
-        <v>510</v>
+      <c r="H4" s="17" t="s">
+        <v>509</v>
+      </c>
+      <c r="I4" s="15">
+        <v>600</v>
       </c>
       <c r="J4" s="15">
-        <v>1800</v>
+        <v>50</v>
       </c>
       <c r="K4" s="15">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="L4" s="15">
-        <v>75</v>
-      </c>
-      <c r="M4" s="15">
         <v>115</v>
       </c>
+      <c r="M4" s="17" t="s">
+        <v>182</v>
+      </c>
       <c r="N4" s="17" t="s">
-        <v>183</v>
+        <v>218</v>
       </c>
       <c r="O4" s="17" t="s">
-        <v>219</v>
+        <v>341</v>
       </c>
       <c r="P4" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="R4" s="17" t="s">
         <v>342</v>
       </c>
-      <c r="Q4" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="R4" s="17" t="s">
-        <v>249</v>
-      </c>
       <c r="S4" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="T4" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="U4" s="17" t="s">
         <v>343</v>
       </c>
-      <c r="T4" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="U4" s="17" t="s">
-        <v>234</v>
-      </c>
-      <c r="V4" s="17" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="45">
+    </row>
+    <row r="5" spans="1:21" ht="45">
       <c r="A5" s="15" t="s">
         <v>91</v>
       </c>
@@ -6621,56 +6606,53 @@
       <c r="F5" s="15">
         <v>50</v>
       </c>
-      <c r="G5" s="15">
-        <v>4</v>
-      </c>
-      <c r="H5" s="16">
+      <c r="G5" s="16">
         <v>720</v>
       </c>
-      <c r="I5" s="17" t="s">
-        <v>511</v>
+      <c r="H5" s="17" t="s">
+        <v>510</v>
+      </c>
+      <c r="I5" s="15">
+        <v>800</v>
       </c>
       <c r="J5" s="15">
-        <v>2400</v>
+        <v>130</v>
       </c>
       <c r="K5" s="15">
-        <v>130</v>
+        <v>195</v>
       </c>
       <c r="L5" s="15">
+        <v>300</v>
+      </c>
+      <c r="M5" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="N5" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="O5" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="P5" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="M5" s="15">
-        <v>300</v>
-      </c>
-      <c r="N5" s="17" t="s">
-        <v>184</v>
-      </c>
-      <c r="O5" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="P5" s="17" t="s">
+      <c r="Q5" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="R5" s="17" t="s">
         <v>345</v>
       </c>
-      <c r="Q5" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="R5" s="17" t="s">
-        <v>250</v>
-      </c>
       <c r="S5" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="T5" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="U5" s="17" t="s">
         <v>346</v>
       </c>
-      <c r="T5" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="U5" s="17" t="s">
-        <v>235</v>
-      </c>
-      <c r="V5" s="17" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="45">
+    </row>
+    <row r="6" spans="1:21" ht="45">
       <c r="A6" s="15" t="s">
         <v>89</v>
       </c>
@@ -6689,56 +6671,53 @@
       <c r="F6" s="15">
         <v>50</v>
       </c>
-      <c r="G6" s="15">
-        <v>4</v>
-      </c>
-      <c r="H6" s="16">
+      <c r="G6" s="16">
         <v>1202</v>
       </c>
-      <c r="I6" s="17" t="s">
-        <v>512</v>
+      <c r="H6" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="I6" s="15">
+        <v>1000</v>
       </c>
       <c r="J6" s="15">
-        <v>3000</v>
+        <v>215</v>
       </c>
       <c r="K6" s="15">
-        <v>215</v>
+        <v>325</v>
       </c>
       <c r="L6" s="15">
-        <v>325</v>
-      </c>
-      <c r="M6" s="15">
         <v>505</v>
       </c>
+      <c r="M6" s="17" t="s">
+        <v>184</v>
+      </c>
       <c r="N6" s="17" t="s">
-        <v>185</v>
+        <v>220</v>
       </c>
       <c r="O6" s="17" t="s">
-        <v>221</v>
+        <v>347</v>
       </c>
       <c r="P6" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q6" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="R6" s="17" t="s">
         <v>348</v>
       </c>
-      <c r="Q6" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="R6" s="17" t="s">
-        <v>251</v>
-      </c>
       <c r="S6" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="T6" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="U6" s="17" t="s">
         <v>349</v>
       </c>
-      <c r="T6" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="U6" s="17" t="s">
-        <v>236</v>
-      </c>
-      <c r="V6" s="17" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="45">
+    </row>
+    <row r="7" spans="1:21" ht="45">
       <c r="A7" s="15" t="s">
         <v>92</v>
       </c>
@@ -6757,56 +6736,53 @@
       <c r="F7" s="15">
         <v>50</v>
       </c>
-      <c r="G7" s="15">
-        <v>4</v>
-      </c>
-      <c r="H7" s="16">
+      <c r="G7" s="16">
         <v>1652</v>
       </c>
-      <c r="I7" s="17" t="s">
-        <v>513</v>
+      <c r="H7" s="17" t="s">
+        <v>512</v>
+      </c>
+      <c r="I7" s="15">
+        <v>1200</v>
       </c>
       <c r="J7" s="15">
-        <v>3600</v>
+        <v>295</v>
       </c>
       <c r="K7" s="15">
-        <v>295</v>
+        <v>445</v>
       </c>
       <c r="L7" s="15">
-        <v>445</v>
-      </c>
-      <c r="M7" s="15">
         <v>695</v>
       </c>
+      <c r="M7" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="N7" s="17" t="s">
-        <v>186</v>
+        <v>221</v>
       </c>
       <c r="O7" s="17" t="s">
-        <v>222</v>
+        <v>350</v>
       </c>
       <c r="P7" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q7" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="R7" s="17" t="s">
         <v>351</v>
       </c>
-      <c r="Q7" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="R7" s="17" t="s">
-        <v>252</v>
-      </c>
       <c r="S7" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="T7" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="U7" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="T7" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="U7" s="17" t="s">
-        <v>237</v>
-      </c>
-      <c r="V7" s="17" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="45">
+    </row>
+    <row r="8" spans="1:21" ht="45">
       <c r="A8" s="15" t="s">
         <v>147</v>
       </c>
@@ -6825,56 +6801,53 @@
       <c r="F8" s="15">
         <v>100</v>
       </c>
-      <c r="G8" s="15">
-        <v>6</v>
-      </c>
-      <c r="H8" s="16">
+      <c r="G8" s="16">
         <v>3602</v>
       </c>
-      <c r="I8" s="17" t="s">
-        <v>514</v>
+      <c r="H8" s="17" t="s">
+        <v>513</v>
+      </c>
+      <c r="I8" s="15">
+        <v>1400</v>
       </c>
       <c r="J8" s="15">
-        <v>4200</v>
+        <v>645</v>
       </c>
       <c r="K8" s="15">
-        <v>645</v>
+        <v>970</v>
       </c>
       <c r="L8" s="15">
-        <v>970</v>
-      </c>
-      <c r="M8" s="15">
         <v>1515</v>
       </c>
+      <c r="M8" s="17" t="s">
+        <v>275</v>
+      </c>
       <c r="N8" s="17" t="s">
-        <v>276</v>
+        <v>302</v>
       </c>
       <c r="O8" s="17" t="s">
-        <v>303</v>
+        <v>353</v>
       </c>
       <c r="P8" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q8" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="R8" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="Q8" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="R8" s="17" t="s">
-        <v>312</v>
-      </c>
       <c r="S8" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="T8" s="17" t="s">
+        <v>320</v>
+      </c>
+      <c r="U8" s="17" t="s">
         <v>355</v>
       </c>
-      <c r="T8" s="17" t="s">
-        <v>294</v>
-      </c>
-      <c r="U8" s="17" t="s">
-        <v>321</v>
-      </c>
-      <c r="V8" s="17" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="45">
+    </row>
+    <row r="9" spans="1:21" ht="45">
       <c r="A9" s="15" t="s">
         <v>93</v>
       </c>
@@ -6893,56 +6866,53 @@
       <c r="F9" s="15">
         <v>100</v>
       </c>
-      <c r="G9" s="15">
-        <v>6</v>
-      </c>
-      <c r="H9" s="16">
+      <c r="G9" s="16">
         <v>4602</v>
       </c>
-      <c r="I9" s="17" t="s">
-        <v>515</v>
+      <c r="H9" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="I9" s="15">
+        <v>1600</v>
       </c>
       <c r="J9" s="15">
-        <v>4800</v>
+        <v>825</v>
       </c>
       <c r="K9" s="15">
-        <v>825</v>
+        <v>1240</v>
       </c>
       <c r="L9" s="15">
-        <v>1240</v>
-      </c>
-      <c r="M9" s="15">
         <v>1935</v>
       </c>
+      <c r="M9" s="17" t="s">
+        <v>186</v>
+      </c>
       <c r="N9" s="17" t="s">
-        <v>187</v>
+        <v>222</v>
       </c>
       <c r="O9" s="17" t="s">
-        <v>223</v>
+        <v>356</v>
       </c>
       <c r="P9" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q9" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="R9" s="17" t="s">
         <v>357</v>
       </c>
-      <c r="Q9" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="R9" s="17" t="s">
-        <v>253</v>
-      </c>
       <c r="S9" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="T9" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="U9" s="17" t="s">
         <v>358</v>
       </c>
-      <c r="T9" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="U9" s="17" t="s">
-        <v>238</v>
-      </c>
-      <c r="V9" s="17" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="45">
+    </row>
+    <row r="10" spans="1:21" ht="45">
       <c r="A10" s="15" t="s">
         <v>88</v>
       </c>
@@ -6961,56 +6931,53 @@
       <c r="F10" s="15">
         <v>100</v>
       </c>
-      <c r="G10" s="15">
-        <v>6</v>
-      </c>
-      <c r="H10" s="16">
+      <c r="G10" s="16">
         <v>5720</v>
       </c>
-      <c r="I10" s="17" t="s">
-        <v>516</v>
+      <c r="H10" s="17" t="s">
+        <v>515</v>
+      </c>
+      <c r="I10" s="15">
+        <v>2000</v>
       </c>
       <c r="J10" s="15">
-        <v>6000</v>
+        <v>1030</v>
       </c>
       <c r="K10" s="15">
-        <v>1030</v>
+        <v>1545</v>
       </c>
       <c r="L10" s="15">
-        <v>1545</v>
-      </c>
-      <c r="M10" s="15">
         <v>2400</v>
       </c>
+      <c r="M10" s="17" t="s">
+        <v>276</v>
+      </c>
       <c r="N10" s="17" t="s">
-        <v>277</v>
+        <v>303</v>
       </c>
       <c r="O10" s="17" t="s">
-        <v>304</v>
+        <v>359</v>
       </c>
       <c r="P10" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q10" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="R10" s="17" t="s">
         <v>360</v>
       </c>
-      <c r="Q10" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="R10" s="17" t="s">
-        <v>313</v>
-      </c>
       <c r="S10" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="T10" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="U10" s="17" t="s">
         <v>361</v>
       </c>
-      <c r="T10" s="17" t="s">
-        <v>295</v>
-      </c>
-      <c r="U10" s="17" t="s">
-        <v>322</v>
-      </c>
-      <c r="V10" s="17" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="45">
+    </row>
+    <row r="11" spans="1:21" ht="45">
       <c r="A11" s="15" t="s">
         <v>87</v>
       </c>
@@ -7029,56 +6996,53 @@
       <c r="F11" s="15">
         <v>100</v>
       </c>
-      <c r="G11" s="15">
-        <v>6</v>
-      </c>
-      <c r="H11" s="16">
+      <c r="G11" s="16">
         <v>10320</v>
       </c>
-      <c r="I11" s="17" t="s">
-        <v>517</v>
+      <c r="H11" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="I11" s="15">
+        <v>2400</v>
       </c>
       <c r="J11" s="15">
-        <v>7200</v>
+        <v>1545</v>
       </c>
       <c r="K11" s="15">
-        <v>1545</v>
+        <v>2320</v>
       </c>
       <c r="L11" s="15">
-        <v>2320</v>
-      </c>
-      <c r="M11" s="15">
         <v>3610</v>
       </c>
+      <c r="M11" s="17" t="s">
+        <v>148</v>
+      </c>
       <c r="N11" s="17" t="s">
-        <v>148</v>
+        <v>223</v>
       </c>
       <c r="O11" s="17" t="s">
-        <v>224</v>
+        <v>362</v>
       </c>
       <c r="P11" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q11" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="R11" s="17" t="s">
         <v>363</v>
       </c>
-      <c r="Q11" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="R11" s="17" t="s">
-        <v>254</v>
-      </c>
       <c r="S11" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="T11" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="U11" s="17" t="s">
         <v>364</v>
       </c>
-      <c r="T11" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="U11" s="17" t="s">
-        <v>239</v>
-      </c>
-      <c r="V11" s="17" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="45">
+    </row>
+    <row r="12" spans="1:21" ht="45">
       <c r="A12" s="15" t="s">
         <v>86</v>
       </c>
@@ -7097,56 +7061,53 @@
       <c r="F12" s="15">
         <v>100</v>
       </c>
-      <c r="G12" s="15">
-        <v>6</v>
-      </c>
-      <c r="H12" s="16">
+      <c r="G12" s="16">
         <v>12300</v>
       </c>
-      <c r="I12" s="17" t="s">
-        <v>518</v>
+      <c r="H12" s="17" t="s">
+        <v>517</v>
+      </c>
+      <c r="I12" s="15">
+        <v>3200</v>
       </c>
       <c r="J12" s="15">
-        <v>9600</v>
+        <v>1845</v>
       </c>
       <c r="K12" s="15">
-        <v>1845</v>
+        <v>2765</v>
       </c>
       <c r="L12" s="15">
-        <v>2765</v>
-      </c>
-      <c r="M12" s="15">
         <v>4305</v>
       </c>
+      <c r="M12" s="17" t="s">
+        <v>277</v>
+      </c>
       <c r="N12" s="17" t="s">
-        <v>278</v>
+        <v>304</v>
       </c>
       <c r="O12" s="17" t="s">
-        <v>305</v>
+        <v>365</v>
       </c>
       <c r="P12" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q12" s="17" t="s">
+        <v>313</v>
+      </c>
+      <c r="R12" s="17" t="s">
         <v>366</v>
       </c>
-      <c r="Q12" s="17" t="s">
-        <v>287</v>
-      </c>
-      <c r="R12" s="17" t="s">
-        <v>314</v>
-      </c>
       <c r="S12" s="17" t="s">
+        <v>295</v>
+      </c>
+      <c r="T12" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="U12" s="17" t="s">
         <v>367</v>
       </c>
-      <c r="T12" s="17" t="s">
-        <v>296</v>
-      </c>
-      <c r="U12" s="17" t="s">
-        <v>323</v>
-      </c>
-      <c r="V12" s="17" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" ht="45">
+    </row>
+    <row r="13" spans="1:21" ht="45">
       <c r="A13" s="15" t="s">
         <v>94</v>
       </c>
@@ -7165,56 +7126,53 @@
       <c r="F13" s="15">
         <v>100</v>
       </c>
-      <c r="G13" s="15">
-        <v>6</v>
-      </c>
-      <c r="H13" s="16">
+      <c r="G13" s="16">
         <v>14400</v>
       </c>
-      <c r="I13" s="17" t="s">
-        <v>519</v>
+      <c r="H13" s="17" t="s">
+        <v>518</v>
+      </c>
+      <c r="I13" s="15">
+        <v>4200</v>
       </c>
       <c r="J13" s="15">
-        <v>12600</v>
+        <v>2160</v>
       </c>
       <c r="K13" s="15">
-        <v>2160</v>
+        <v>3240</v>
       </c>
       <c r="L13" s="15">
-        <v>3240</v>
-      </c>
-      <c r="M13" s="15">
         <v>5040</v>
       </c>
+      <c r="M13" s="17" t="s">
+        <v>187</v>
+      </c>
       <c r="N13" s="17" t="s">
-        <v>188</v>
+        <v>224</v>
       </c>
       <c r="O13" s="17" t="s">
-        <v>225</v>
+        <v>368</v>
       </c>
       <c r="P13" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q13" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="R13" s="17" t="s">
         <v>369</v>
       </c>
-      <c r="Q13" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="R13" s="17" t="s">
-        <v>255</v>
-      </c>
       <c r="S13" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="T13" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="U13" s="17" t="s">
         <v>370</v>
       </c>
-      <c r="T13" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="U13" s="17" t="s">
-        <v>240</v>
-      </c>
-      <c r="V13" s="17" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="45">
+    </row>
+    <row r="14" spans="1:21" ht="45">
       <c r="A14" s="15" t="s">
         <v>151</v>
       </c>
@@ -7233,56 +7191,53 @@
       <c r="F14" s="15">
         <v>150</v>
       </c>
-      <c r="G14" s="15">
-        <v>8</v>
-      </c>
-      <c r="H14" s="16">
+      <c r="G14" s="16">
         <v>22400</v>
       </c>
-      <c r="I14" s="17" t="s">
-        <v>520</v>
+      <c r="H14" s="17" t="s">
+        <v>519</v>
+      </c>
+      <c r="I14" s="15">
+        <v>6000</v>
       </c>
       <c r="J14" s="15">
-        <v>18000</v>
+        <v>3020</v>
       </c>
       <c r="K14" s="15">
-        <v>3020</v>
+        <v>4535</v>
       </c>
       <c r="L14" s="15">
-        <v>4535</v>
-      </c>
-      <c r="M14" s="15">
         <v>7055</v>
       </c>
+      <c r="M14" s="17" t="s">
+        <v>278</v>
+      </c>
       <c r="N14" s="17" t="s">
-        <v>279</v>
+        <v>305</v>
       </c>
       <c r="O14" s="17" t="s">
-        <v>306</v>
+        <v>371</v>
       </c>
       <c r="P14" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q14" s="17" t="s">
+        <v>314</v>
+      </c>
+      <c r="R14" s="17" t="s">
         <v>372</v>
       </c>
-      <c r="Q14" s="17" t="s">
-        <v>288</v>
-      </c>
-      <c r="R14" s="17" t="s">
-        <v>315</v>
-      </c>
       <c r="S14" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="T14" s="17" t="s">
+        <v>323</v>
+      </c>
+      <c r="U14" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="T14" s="17" t="s">
-        <v>297</v>
-      </c>
-      <c r="U14" s="17" t="s">
-        <v>324</v>
-      </c>
-      <c r="V14" s="17" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="45">
+    </row>
+    <row r="15" spans="1:21" ht="45">
       <c r="A15" s="15" t="s">
         <v>95</v>
       </c>
@@ -7301,56 +7256,53 @@
       <c r="F15" s="15">
         <v>150</v>
       </c>
-      <c r="G15" s="15">
-        <v>8</v>
-      </c>
-      <c r="H15" s="16">
+      <c r="G15" s="16">
         <v>24800</v>
       </c>
-      <c r="I15" s="17" t="s">
-        <v>521</v>
+      <c r="H15" s="17" t="s">
+        <v>520</v>
+      </c>
+      <c r="I15" s="15">
+        <v>7500</v>
       </c>
       <c r="J15" s="15">
-        <v>22500</v>
+        <v>3345</v>
       </c>
       <c r="K15" s="15">
-        <v>3345</v>
+        <v>5020</v>
       </c>
       <c r="L15" s="15">
-        <v>5020</v>
-      </c>
-      <c r="M15" s="15">
         <v>7810</v>
       </c>
+      <c r="M15" s="17" t="s">
+        <v>188</v>
+      </c>
       <c r="N15" s="17" t="s">
-        <v>189</v>
+        <v>225</v>
       </c>
       <c r="O15" s="17" t="s">
-        <v>226</v>
+        <v>374</v>
       </c>
       <c r="P15" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q15" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="R15" s="17" t="s">
         <v>375</v>
       </c>
-      <c r="Q15" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="R15" s="17" t="s">
-        <v>256</v>
-      </c>
       <c r="S15" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="T15" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="U15" s="17" t="s">
         <v>376</v>
       </c>
-      <c r="T15" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="U15" s="17" t="s">
-        <v>241</v>
-      </c>
-      <c r="V15" s="17" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" ht="45">
+    </row>
+    <row r="16" spans="1:21" ht="45">
       <c r="A16" s="15" t="s">
         <v>85</v>
       </c>
@@ -7369,56 +7321,53 @@
       <c r="F16" s="15">
         <v>150</v>
       </c>
-      <c r="G16" s="15">
-        <v>8</v>
-      </c>
-      <c r="H16" s="16">
+      <c r="G16" s="16">
         <v>28000</v>
       </c>
-      <c r="I16" s="17" t="s">
-        <v>522</v>
+      <c r="H16" s="17" t="s">
+        <v>521</v>
+      </c>
+      <c r="I16" s="15">
+        <v>10500</v>
       </c>
       <c r="J16" s="15">
-        <v>31500</v>
+        <v>3780</v>
       </c>
       <c r="K16" s="15">
-        <v>3780</v>
+        <v>5670</v>
       </c>
       <c r="L16" s="15">
-        <v>5670</v>
-      </c>
-      <c r="M16" s="15">
         <v>8820</v>
       </c>
+      <c r="M16" s="17" t="s">
+        <v>279</v>
+      </c>
       <c r="N16" s="17" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="O16" s="17" t="s">
-        <v>307</v>
+        <v>377</v>
       </c>
       <c r="P16" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q16" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="R16" s="17" t="s">
         <v>378</v>
       </c>
-      <c r="Q16" s="17" t="s">
-        <v>289</v>
-      </c>
-      <c r="R16" s="17" t="s">
-        <v>316</v>
-      </c>
       <c r="S16" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="T16" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="U16" s="17" t="s">
         <v>379</v>
       </c>
-      <c r="T16" s="17" t="s">
-        <v>298</v>
-      </c>
-      <c r="U16" s="17" t="s">
-        <v>325</v>
-      </c>
-      <c r="V16" s="17" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" ht="45">
+    </row>
+    <row r="17" spans="1:21" ht="45">
       <c r="A17" s="15" t="s">
         <v>84</v>
       </c>
@@ -7437,56 +7386,53 @@
       <c r="F17" s="15">
         <v>150</v>
       </c>
-      <c r="G17" s="15">
-        <v>8</v>
-      </c>
-      <c r="H17" s="16">
+      <c r="G17" s="16">
         <v>39000</v>
       </c>
-      <c r="I17" s="17" t="s">
-        <v>523</v>
+      <c r="H17" s="17" t="s">
+        <v>522</v>
+      </c>
+      <c r="I17" s="15">
+        <v>12800</v>
       </c>
       <c r="J17" s="15">
-        <v>38400</v>
+        <v>4910</v>
       </c>
       <c r="K17" s="15">
-        <v>4910</v>
+        <v>7370</v>
       </c>
       <c r="L17" s="15">
-        <v>7370</v>
-      </c>
-      <c r="M17" s="15">
         <v>11465</v>
       </c>
+      <c r="M17" s="17" t="s">
+        <v>152</v>
+      </c>
       <c r="N17" s="17" t="s">
-        <v>152</v>
+        <v>226</v>
       </c>
       <c r="O17" s="17" t="s">
-        <v>227</v>
+        <v>380</v>
       </c>
       <c r="P17" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q17" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="R17" s="17" t="s">
         <v>381</v>
       </c>
-      <c r="Q17" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="R17" s="17" t="s">
-        <v>257</v>
-      </c>
       <c r="S17" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="T17" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="U17" s="17" t="s">
         <v>382</v>
       </c>
-      <c r="T17" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="U17" s="17" t="s">
-        <v>242</v>
-      </c>
-      <c r="V17" s="17" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" ht="45">
+    </row>
+    <row r="18" spans="1:21" ht="45">
       <c r="A18" s="15" t="s">
         <v>83</v>
       </c>
@@ -7505,56 +7451,53 @@
       <c r="F18" s="15">
         <v>150</v>
       </c>
-      <c r="G18" s="15">
-        <v>8</v>
-      </c>
-      <c r="H18" s="16">
+      <c r="G18" s="16">
         <v>43000</v>
       </c>
-      <c r="I18" s="17" t="s">
-        <v>524</v>
+      <c r="H18" s="17" t="s">
+        <v>523</v>
+      </c>
+      <c r="I18" s="15">
+        <v>18700</v>
       </c>
       <c r="J18" s="15">
-        <v>56100</v>
+        <v>5415</v>
       </c>
       <c r="K18" s="15">
-        <v>5415</v>
+        <v>8125</v>
       </c>
       <c r="L18" s="15">
-        <v>8125</v>
-      </c>
-      <c r="M18" s="15">
         <v>12640</v>
       </c>
+      <c r="M18" s="17" t="s">
+        <v>280</v>
+      </c>
       <c r="N18" s="17" t="s">
-        <v>281</v>
+        <v>307</v>
       </c>
       <c r="O18" s="17" t="s">
-        <v>308</v>
+        <v>383</v>
       </c>
       <c r="P18" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q18" s="17" t="s">
+        <v>316</v>
+      </c>
+      <c r="R18" s="17" t="s">
         <v>384</v>
       </c>
-      <c r="Q18" s="17" t="s">
-        <v>290</v>
-      </c>
-      <c r="R18" s="17" t="s">
-        <v>317</v>
-      </c>
       <c r="S18" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="T18" s="17" t="s">
+        <v>325</v>
+      </c>
+      <c r="U18" s="17" t="s">
         <v>385</v>
       </c>
-      <c r="T18" s="17" t="s">
-        <v>299</v>
-      </c>
-      <c r="U18" s="17" t="s">
-        <v>326</v>
-      </c>
-      <c r="V18" s="17" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" ht="45">
+    </row>
+    <row r="19" spans="1:21" ht="45">
       <c r="A19" s="15" t="s">
         <v>96</v>
       </c>
@@ -7573,56 +7516,53 @@
       <c r="F19" s="15">
         <v>150</v>
       </c>
-      <c r="G19" s="15">
-        <v>8</v>
-      </c>
-      <c r="H19" s="12">
+      <c r="G19" s="12">
         <v>48000</v>
       </c>
-      <c r="I19" s="17" t="s">
-        <v>525</v>
+      <c r="H19" s="17" t="s">
+        <v>524</v>
+      </c>
+      <c r="I19" s="15">
+        <v>22500</v>
       </c>
       <c r="J19" s="15">
-        <v>67500</v>
+        <v>6045</v>
       </c>
       <c r="K19" s="15">
-        <v>6045</v>
+        <v>9070</v>
       </c>
       <c r="L19" s="15">
-        <v>9070</v>
-      </c>
-      <c r="M19" s="15">
         <v>14110</v>
       </c>
+      <c r="M19" s="17" t="s">
+        <v>189</v>
+      </c>
       <c r="N19" s="17" t="s">
-        <v>190</v>
+        <v>227</v>
       </c>
       <c r="O19" s="17" t="s">
-        <v>228</v>
+        <v>386</v>
       </c>
       <c r="P19" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q19" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="R19" s="17" t="s">
         <v>387</v>
       </c>
-      <c r="Q19" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="R19" s="17" t="s">
-        <v>258</v>
-      </c>
       <c r="S19" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="T19" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="U19" s="17" t="s">
         <v>388</v>
       </c>
-      <c r="T19" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="U19" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="V19" s="17" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" ht="45">
+    </row>
+    <row r="20" spans="1:21" ht="45">
       <c r="A20" s="15" t="s">
         <v>155</v>
       </c>
@@ -7641,56 +7581,53 @@
       <c r="F20" s="15">
         <v>200</v>
       </c>
-      <c r="G20" s="15">
-        <v>10</v>
-      </c>
-      <c r="H20" s="12">
+      <c r="G20" s="12">
         <v>78000</v>
       </c>
-      <c r="I20" s="17" t="s">
-        <v>526</v>
+      <c r="H20" s="17" t="s">
+        <v>525</v>
+      </c>
+      <c r="I20" s="15">
+        <v>32700</v>
       </c>
       <c r="J20" s="15">
-        <v>98100</v>
+        <v>7485</v>
       </c>
       <c r="K20" s="15">
-        <v>7485</v>
+        <v>11230</v>
       </c>
       <c r="L20" s="15">
-        <v>11230</v>
-      </c>
-      <c r="M20" s="15">
         <v>17470</v>
       </c>
+      <c r="M20" s="17" t="s">
+        <v>281</v>
+      </c>
       <c r="N20" s="17" t="s">
-        <v>282</v>
+        <v>308</v>
       </c>
       <c r="O20" s="17" t="s">
-        <v>309</v>
+        <v>389</v>
       </c>
       <c r="P20" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q20" s="17" t="s">
+        <v>317</v>
+      </c>
+      <c r="R20" s="17" t="s">
         <v>390</v>
       </c>
-      <c r="Q20" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="R20" s="17" t="s">
-        <v>318</v>
-      </c>
       <c r="S20" s="17" t="s">
+        <v>299</v>
+      </c>
+      <c r="T20" s="17" t="s">
+        <v>326</v>
+      </c>
+      <c r="U20" s="17" t="s">
         <v>391</v>
       </c>
-      <c r="T20" s="17" t="s">
-        <v>300</v>
-      </c>
-      <c r="U20" s="17" t="s">
-        <v>327</v>
-      </c>
-      <c r="V20" s="17" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" ht="45">
+    </row>
+    <row r="21" spans="1:21" ht="45">
       <c r="A21" s="15" t="s">
         <v>97</v>
       </c>
@@ -7709,56 +7646,53 @@
       <c r="F21" s="15">
         <v>200</v>
       </c>
-      <c r="G21" s="15">
-        <v>10</v>
-      </c>
-      <c r="H21" s="12">
+      <c r="G21" s="12">
         <v>85500</v>
       </c>
-      <c r="I21" s="17" t="s">
-        <v>527</v>
+      <c r="H21" s="17" t="s">
+        <v>526</v>
+      </c>
+      <c r="I21" s="15">
+        <v>39300</v>
       </c>
       <c r="J21" s="15">
-        <v>117900</v>
+        <v>8205</v>
       </c>
       <c r="K21" s="15">
-        <v>8205</v>
+        <v>12310</v>
       </c>
       <c r="L21" s="15">
-        <v>12310</v>
-      </c>
-      <c r="M21" s="15">
         <v>19150</v>
       </c>
+      <c r="M21" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="N21" s="17" t="s">
-        <v>191</v>
+        <v>228</v>
       </c>
       <c r="O21" s="17" t="s">
-        <v>229</v>
+        <v>392</v>
       </c>
       <c r="P21" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q21" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="R21" s="17" t="s">
         <v>393</v>
       </c>
-      <c r="Q21" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="R21" s="17" t="s">
-        <v>259</v>
-      </c>
       <c r="S21" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="T21" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="U21" s="17" t="s">
         <v>394</v>
       </c>
-      <c r="T21" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="U21" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="V21" s="17" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" ht="45">
+    </row>
+    <row r="22" spans="1:21" ht="45">
       <c r="A22" s="15" t="s">
         <v>98</v>
       </c>
@@ -7777,56 +7711,53 @@
       <c r="F22" s="15">
         <v>200</v>
       </c>
-      <c r="G22" s="15">
-        <v>10</v>
-      </c>
-      <c r="H22" s="12">
+      <c r="G22" s="12">
         <v>122000</v>
       </c>
-      <c r="I22" s="17" t="s">
-        <v>528</v>
-      </c>
-      <c r="J22" s="15">
-        <v>170100</v>
+      <c r="H22" s="17" t="s">
+        <v>527</v>
+      </c>
+      <c r="I22" s="15">
+        <v>56700</v>
+      </c>
+      <c r="J22" s="12">
+        <v>9880</v>
       </c>
       <c r="K22" s="12">
-        <v>9880</v>
+        <v>14820</v>
       </c>
       <c r="L22" s="12">
-        <v>14820</v>
-      </c>
-      <c r="M22" s="12">
         <v>23055</v>
       </c>
+      <c r="M22" s="17" t="s">
+        <v>282</v>
+      </c>
       <c r="N22" s="17" t="s">
-        <v>283</v>
+        <v>309</v>
       </c>
       <c r="O22" s="17" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="P22" s="17" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q22" s="17" t="s">
+        <v>318</v>
+      </c>
+      <c r="R22" s="17" t="s">
         <v>396</v>
       </c>
-      <c r="Q22" s="17" t="s">
-        <v>292</v>
-      </c>
-      <c r="R22" s="17" t="s">
-        <v>319</v>
-      </c>
       <c r="S22" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="T22" s="17" t="s">
+        <v>327</v>
+      </c>
+      <c r="U22" s="17" t="s">
         <v>397</v>
       </c>
-      <c r="T22" s="17" t="s">
-        <v>301</v>
-      </c>
-      <c r="U22" s="17" t="s">
-        <v>328</v>
-      </c>
-      <c r="V22" s="17" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" ht="45">
+    </row>
+    <row r="23" spans="1:21" ht="45">
       <c r="A23" s="15" t="s">
         <v>99</v>
       </c>
@@ -7845,56 +7776,53 @@
       <c r="F23" s="15">
         <v>200</v>
       </c>
-      <c r="G23" s="15">
-        <v>10</v>
-      </c>
-      <c r="H23" s="12">
+      <c r="G23" s="12">
         <v>132000</v>
       </c>
-      <c r="I23" s="22" t="s">
-        <v>529</v>
-      </c>
-      <c r="J23" s="15">
-        <v>204000</v>
+      <c r="H23" s="22" t="s">
+        <v>528</v>
+      </c>
+      <c r="I23" s="15">
+        <v>68000</v>
+      </c>
+      <c r="J23" s="12">
+        <v>10690</v>
       </c>
       <c r="K23" s="12">
-        <v>10690</v>
+        <v>16035</v>
       </c>
       <c r="L23" s="12">
-        <v>16035</v>
-      </c>
-      <c r="M23" s="12">
         <v>24945</v>
       </c>
+      <c r="M23" s="17" t="s">
+        <v>156</v>
+      </c>
       <c r="N23" s="17" t="s">
-        <v>156</v>
+        <v>229</v>
       </c>
       <c r="O23" s="17" t="s">
-        <v>230</v>
+        <v>398</v>
       </c>
       <c r="P23" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q23" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="R23" s="17" t="s">
         <v>399</v>
       </c>
-      <c r="Q23" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="R23" s="17" t="s">
-        <v>260</v>
-      </c>
       <c r="S23" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="T23" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="U23" s="17" t="s">
         <v>400</v>
       </c>
-      <c r="T23" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="U23" s="17" t="s">
-        <v>245</v>
-      </c>
-      <c r="V23" s="17" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" ht="45">
+    </row>
+    <row r="24" spans="1:21" ht="45">
       <c r="A24" s="15" t="s">
         <v>100</v>
       </c>
@@ -7913,56 +7841,53 @@
       <c r="F24" s="15">
         <v>200</v>
       </c>
-      <c r="G24" s="15">
-        <v>10</v>
-      </c>
-      <c r="H24" s="12">
+      <c r="G24" s="12">
         <v>180000</v>
       </c>
-      <c r="I24" s="22" t="s">
-        <v>530</v>
+      <c r="H24" s="22" t="s">
+        <v>529</v>
+      </c>
+      <c r="I24" s="12">
+        <v>80000</v>
       </c>
       <c r="J24" s="12">
-        <v>240000</v>
+        <v>12960</v>
       </c>
       <c r="K24" s="12">
-        <v>12960</v>
+        <v>19440</v>
       </c>
       <c r="L24" s="12">
-        <v>19440</v>
-      </c>
-      <c r="M24" s="12">
         <v>30240</v>
       </c>
-      <c r="N24" s="22" t="s">
-        <v>284</v>
+      <c r="M24" s="22" t="s">
+        <v>283</v>
+      </c>
+      <c r="N24" s="17" t="s">
+        <v>310</v>
       </c>
       <c r="O24" s="17" t="s">
-        <v>311</v>
+        <v>401</v>
       </c>
       <c r="P24" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q24" s="17" t="s">
+        <v>319</v>
+      </c>
+      <c r="R24" s="17" t="s">
         <v>402</v>
       </c>
-      <c r="Q24" s="17" t="s">
-        <v>293</v>
-      </c>
-      <c r="R24" s="17" t="s">
-        <v>320</v>
-      </c>
       <c r="S24" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="T24" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="U24" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="T24" s="17" t="s">
-        <v>302</v>
-      </c>
-      <c r="U24" s="17" t="s">
-        <v>329</v>
-      </c>
-      <c r="V24" s="17" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" ht="45">
+    </row>
+    <row r="25" spans="1:21" ht="45">
       <c r="A25" s="15" t="s">
         <v>101</v>
       </c>
@@ -7982,63 +7907,61 @@
         <v>200</v>
       </c>
       <c r="G25" s="12">
-        <v>10</v>
-      </c>
-      <c r="H25" s="12">
         <v>200000</v>
       </c>
-      <c r="I25" s="12" t="s">
-        <v>531</v>
+      <c r="H25" s="12" t="s">
+        <v>530</v>
+      </c>
+      <c r="I25" s="12">
+        <v>100000</v>
       </c>
       <c r="J25" s="12">
-        <v>300000</v>
+        <v>14400</v>
       </c>
       <c r="K25" s="12">
-        <v>14400</v>
+        <v>21600</v>
       </c>
       <c r="L25" s="12">
-        <v>21600</v>
-      </c>
-      <c r="M25" s="12">
         <v>33600</v>
       </c>
+      <c r="M25" s="22" t="s">
+        <v>191</v>
+      </c>
       <c r="N25" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="O25" s="22" t="s">
-        <v>231</v>
+        <v>230</v>
+      </c>
+      <c r="O25" s="17" t="s">
+        <v>404</v>
       </c>
       <c r="P25" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q25" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="R25" s="17" t="s">
         <v>405</v>
       </c>
-      <c r="Q25" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="R25" s="17" t="s">
-        <v>261</v>
-      </c>
       <c r="S25" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="T25" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="U25" s="17" t="s">
         <v>406</v>
       </c>
-      <c r="T25" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="U25" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="V25" s="17" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" ht="20" customHeight="1">
+    </row>
+    <row r="27" spans="1:21" ht="20" customHeight="1">
+      <c r="N27" s="15"/>
       <c r="O27" s="15"/>
       <c r="P27" s="15"/>
       <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
+      <c r="S27" s="15"/>
       <c r="T27" s="15"/>
-      <c r="U27" s="15"/>
-    </row>
-    <row r="28" spans="1:22" ht="20" customHeight="1">
+    </row>
+    <row r="28" spans="1:21" ht="20" customHeight="1">
+      <c r="N28" s="15"/>
       <c r="O28" s="15"/>
       <c r="P28" s="15"/>
       <c r="Q28" s="15"/>
@@ -8046,13 +7969,12 @@
       <c r="S28" s="15"/>
       <c r="T28" s="15"/>
       <c r="U28" s="15"/>
-      <c r="V28" s="15"/>
-    </row>
-    <row r="29" spans="1:22" ht="20" customHeight="1">
-      <c r="O29" s="15"/>
-      <c r="S29" s="15"/>
+    </row>
+    <row r="29" spans="1:21" ht="20" customHeight="1">
+      <c r="N29" s="15"/>
+      <c r="R29" s="15"/>
+      <c r="T29" s="15"/>
       <c r="U29" s="15"/>
-      <c r="V29" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
@@ -8085,16 +8007,16 @@
   <sheetData>
     <row r="1" spans="1:6" s="19" customFormat="1">
       <c r="A1" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" s="23" t="s">
         <v>268</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>270</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>273</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>269</v>
       </c>
       <c r="F1" s="20"/>
     </row>
@@ -8103,13 +8025,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30">
@@ -8117,13 +8039,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30">
@@ -8131,13 +8053,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30">
@@ -8145,13 +8067,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30">
@@ -8159,13 +8081,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30">
@@ -8173,13 +8095,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30">
@@ -8187,13 +8109,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30">
@@ -8201,13 +8123,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30">
@@ -8215,13 +8137,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30">
@@ -8229,13 +8151,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="45">
@@ -8243,13 +8165,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="45">
@@ -8257,13 +8179,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45">
@@ -8271,13 +8193,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="45">
@@ -8285,13 +8207,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="45">
@@ -8299,13 +8221,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="45">
@@ -8313,13 +8235,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="45">
@@ -8327,13 +8249,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="45">
@@ -8341,13 +8263,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="45">
@@ -8355,13 +8277,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="45">
@@ -8369,13 +8291,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="60">
@@ -8383,13 +8305,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="60">
@@ -8397,13 +8319,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="60">
@@ -8411,13 +8333,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="60">
@@ -8425,13 +8347,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="60">
@@ -8439,13 +8361,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="60">
@@ -8453,13 +8375,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="60">
@@ -8467,13 +8389,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="60">
@@ -8481,13 +8403,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="60">
@@ -8495,13 +8417,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="60">
@@ -8509,13 +8431,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="75">
@@ -8523,13 +8445,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="30">
@@ -8537,13 +8459,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30">
@@ -8551,13 +8473,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30">
@@ -8565,13 +8487,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="30">
@@ -8579,13 +8501,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="30">
@@ -8593,13 +8515,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="30">
@@ -8607,13 +8529,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="30">
@@ -8621,13 +8543,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="30">
@@ -8635,13 +8557,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="48" customHeight="1">
@@ -8649,13 +8571,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>